<commit_message>
added functionality for grouping state abbreviations and full proper names
</commit_message>
<xml_diff>
--- a/JeopardyGameBoxScores.xlsx
+++ b/JeopardyGameBoxScores.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2171" uniqueCount="2171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2148" uniqueCount="2148">
   <si>
     <t>EpisodeNumber</t>
   </si>
@@ -5401,9 +5401,6 @@
     <t>Ocean City</t>
   </si>
   <si>
-    <t>NJ</t>
-  </si>
-  <si>
     <t>MELLO</t>
   </si>
   <si>
@@ -5902,9 +5899,6 @@
     <t>Downey</t>
   </si>
   <si>
-    <t>CA</t>
-  </si>
-  <si>
     <t>Dos</t>
   </si>
   <si>
@@ -5914,9 +5908,6 @@
     <t>Ottawa</t>
   </si>
   <si>
-    <t>Ontario</t>
-  </si>
-  <si>
     <t>5636</t>
   </si>
   <si>
@@ -5932,9 +5923,6 @@
     <t>Dayton</t>
   </si>
   <si>
-    <t>OH</t>
-  </si>
-  <si>
     <t>Jiang</t>
   </si>
   <si>
@@ -5944,9 +5932,6 @@
     <t>Brooklyn</t>
   </si>
   <si>
-    <t>NY</t>
-  </si>
-  <si>
     <t>5631</t>
   </si>
   <si>
@@ -5986,9 +5971,6 @@
     <t>Duluth</t>
   </si>
   <si>
-    <t>GA</t>
-  </si>
-  <si>
     <t>Elliott</t>
   </si>
   <si>
@@ -5998,9 +5980,6 @@
     <t>Originally Derry</t>
   </si>
   <si>
-    <t>NH</t>
-  </si>
-  <si>
     <t>5621</t>
   </si>
   <si>
@@ -6037,9 +6016,6 @@
     <t>Durham</t>
   </si>
   <si>
-    <t>NC</t>
-  </si>
-  <si>
     <t>Feyer</t>
   </si>
   <si>
@@ -6073,9 +6049,6 @@
     <t>Arvada</t>
   </si>
   <si>
-    <t>CO</t>
-  </si>
-  <si>
     <t>5556</t>
   </si>
   <si>
@@ -6091,9 +6064,6 @@
     <t>Grand Rapids</t>
   </si>
   <si>
-    <t>MI</t>
-  </si>
-  <si>
     <t>Gomes</t>
   </si>
   <si>
@@ -6118,9 +6088,6 @@
     <t>Originally Kansas City</t>
   </si>
   <si>
-    <t>KS</t>
-  </si>
-  <si>
     <t>Liao</t>
   </si>
   <si>
@@ -6130,9 +6097,6 @@
     <t>Pittsburgh</t>
   </si>
   <si>
-    <t>PA</t>
-  </si>
-  <si>
     <t>5546</t>
   </si>
   <si>
@@ -6148,9 +6112,6 @@
     <t>North Mankato</t>
   </si>
   <si>
-    <t>MN</t>
-  </si>
-  <si>
     <t>Millat</t>
   </si>
   <si>
@@ -6175,9 +6136,6 @@
     <t>Walla Walla</t>
   </si>
   <si>
-    <t>WA</t>
-  </si>
-  <si>
     <t>Warren</t>
   </si>
   <si>
@@ -6187,9 +6145,6 @@
     <t>Petersburg</t>
   </si>
   <si>
-    <t>IL</t>
-  </si>
-  <si>
     <t>5516</t>
   </si>
   <si>
@@ -6205,9 +6160,6 @@
     <t>Washington</t>
   </si>
   <si>
-    <t>D.c.</t>
-  </si>
-  <si>
     <t>Rau</t>
   </si>
   <si>
@@ -6241,7 +6193,7 @@
     <t>Ames</t>
   </si>
   <si>
-    <t>IA</t>
+    <t>IOWA</t>
   </si>
   <si>
     <t>5506</t>
@@ -6283,9 +6235,6 @@
     <t>Kansas City</t>
   </si>
   <si>
-    <t>MO</t>
-  </si>
-  <si>
     <t>Adams</t>
   </si>
   <si>
@@ -6295,9 +6244,6 @@
     <t>North Weymouth</t>
   </si>
   <si>
-    <t>MA</t>
-  </si>
-  <si>
     <t>5496</t>
   </si>
   <si>
@@ -6352,9 +6298,6 @@
     <t>Baltimore</t>
   </si>
   <si>
-    <t>MD</t>
-  </si>
-  <si>
     <t>Pennant</t>
   </si>
   <si>
@@ -6424,9 +6367,6 @@
     <t>Arlington</t>
   </si>
   <si>
-    <t>VA</t>
-  </si>
-  <si>
     <t>Woodall</t>
   </si>
   <si>
@@ -6436,9 +6376,6 @@
     <t>Fort Smith</t>
   </si>
   <si>
-    <t>AR</t>
-  </si>
-  <si>
     <t>5466</t>
   </si>
   <si>
@@ -6451,9 +6388,6 @@
     <t>Annabel</t>
   </si>
   <si>
-    <t>TX</t>
-  </si>
-  <si>
     <t>Avrahami</t>
   </si>
   <si>
@@ -6500,9 +6434,6 @@
   </si>
   <si>
     <t>Hoover</t>
-  </si>
-  <si>
-    <t>AL</t>
   </si>
   <si>
     <t>5451</t>
@@ -57477,7 +57408,7 @@
         <v>1794</v>
       </c>
       <c r="F905" t="s">
-        <v>1795</v>
+        <v>136</v>
       </c>
       <c r="G905" t="s">
         <v>24</v>
@@ -57580,13 +57511,13 @@
         <v>1791</v>
       </c>
       <c r="C907" t="s">
+        <v>1795</v>
+      </c>
+      <c r="D907" t="s">
         <v>1796</v>
       </c>
-      <c r="D907" t="s">
+      <c r="E907" t="s">
         <v>1797</v>
-      </c>
-      <c r="E907" t="s">
-        <v>1798</v>
       </c>
       <c r="F907" t="s">
         <v>245</v>
@@ -57630,10 +57561,10 @@
     </row>
     <row r="908">
       <c r="A908" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B908" t="s">
         <v>1799</v>
-      </c>
-      <c r="B908" t="s">
-        <v>1800</v>
       </c>
       <c r="C908" t="s">
         <v>1792</v>
@@ -57645,7 +57576,7 @@
         <v>1794</v>
       </c>
       <c r="F908" t="s">
-        <v>1795</v>
+        <v>136</v>
       </c>
       <c r="G908" t="s">
         <v>41</v>
@@ -57686,16 +57617,16 @@
     </row>
     <row r="909">
       <c r="A909" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B909" t="s">
         <v>1799</v>
       </c>
-      <c r="B909" t="s">
+      <c r="C909" t="s">
         <v>1800</v>
       </c>
-      <c r="C909" t="s">
+      <c r="D909" t="s">
         <v>1801</v>
-      </c>
-      <c r="D909" t="s">
-        <v>1802</v>
       </c>
       <c r="E909" t="s">
         <v>272</v>
@@ -57742,10 +57673,10 @@
     </row>
     <row r="910">
       <c r="A910" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B910" t="s">
         <v>1799</v>
-      </c>
-      <c r="B910" t="s">
-        <v>1800</v>
       </c>
       <c r="C910" t="s">
         <v>436</v>
@@ -57798,10 +57729,10 @@
     </row>
     <row r="911">
       <c r="A911" t="s">
+        <v>1802</v>
+      </c>
+      <c r="B911" t="s">
         <v>1803</v>
-      </c>
-      <c r="B911" t="s">
-        <v>1804</v>
       </c>
       <c r="C911" t="s">
         <v>1792</v>
@@ -57813,7 +57744,7 @@
         <v>1794</v>
       </c>
       <c r="F911" t="s">
-        <v>1795</v>
+        <v>136</v>
       </c>
       <c r="G911" t="s">
         <v>41</v>
@@ -57854,19 +57785,19 @@
     </row>
     <row r="912">
       <c r="A912" t="s">
+        <v>1802</v>
+      </c>
+      <c r="B912" t="s">
         <v>1803</v>
       </c>
-      <c r="B912" t="s">
+      <c r="C912" t="s">
         <v>1804</v>
-      </c>
-      <c r="C912" t="s">
-        <v>1805</v>
       </c>
       <c r="D912" t="s">
         <v>102</v>
       </c>
       <c r="E912" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="F912" t="s">
         <v>139</v>
@@ -57910,16 +57841,16 @@
     </row>
     <row r="913">
       <c r="A913" t="s">
+        <v>1802</v>
+      </c>
+      <c r="B913" t="s">
         <v>1803</v>
       </c>
-      <c r="B913" t="s">
-        <v>1804</v>
-      </c>
       <c r="C913" t="s">
+        <v>1806</v>
+      </c>
+      <c r="D913" t="s">
         <v>1807</v>
-      </c>
-      <c r="D913" t="s">
-        <v>1808</v>
       </c>
       <c r="E913" t="s">
         <v>294</v>
@@ -57966,10 +57897,10 @@
     </row>
     <row r="914">
       <c r="A914" t="s">
+        <v>1808</v>
+      </c>
+      <c r="B914" t="s">
         <v>1809</v>
-      </c>
-      <c r="B914" t="s">
-        <v>1810</v>
       </c>
       <c r="C914" t="s">
         <v>1792</v>
@@ -57981,7 +57912,7 @@
         <v>1794</v>
       </c>
       <c r="F914" t="s">
-        <v>1795</v>
+        <v>136</v>
       </c>
       <c r="G914" t="s">
         <v>41</v>
@@ -58022,13 +57953,13 @@
     </row>
     <row r="915">
       <c r="A915" t="s">
+        <v>1808</v>
+      </c>
+      <c r="B915" t="s">
         <v>1809</v>
       </c>
-      <c r="B915" t="s">
+      <c r="C915" t="s">
         <v>1810</v>
-      </c>
-      <c r="C915" t="s">
-        <v>1811</v>
       </c>
       <c r="D915" t="s">
         <v>867</v>
@@ -58078,19 +58009,19 @@
     </row>
     <row r="916">
       <c r="A916" t="s">
+        <v>1808</v>
+      </c>
+      <c r="B916" t="s">
         <v>1809</v>
       </c>
-      <c r="B916" t="s">
-        <v>1810</v>
-      </c>
       <c r="C916" t="s">
+        <v>1811</v>
+      </c>
+      <c r="D916" t="s">
         <v>1812</v>
       </c>
-      <c r="D916" t="s">
+      <c r="E916" t="s">
         <v>1813</v>
-      </c>
-      <c r="E916" t="s">
-        <v>1814</v>
       </c>
       <c r="F916" t="s">
         <v>118</v>
@@ -58134,10 +58065,10 @@
     </row>
     <row r="917">
       <c r="A917" t="s">
+        <v>1814</v>
+      </c>
+      <c r="B917" t="s">
         <v>1815</v>
-      </c>
-      <c r="B917" t="s">
-        <v>1816</v>
       </c>
       <c r="C917" t="s">
         <v>1792</v>
@@ -58149,7 +58080,7 @@
         <v>1794</v>
       </c>
       <c r="F917" t="s">
-        <v>1795</v>
+        <v>136</v>
       </c>
       <c r="G917" t="s">
         <v>41</v>
@@ -58190,16 +58121,16 @@
     </row>
     <row r="918">
       <c r="A918" t="s">
+        <v>1814</v>
+      </c>
+      <c r="B918" t="s">
         <v>1815</v>
       </c>
-      <c r="B918" t="s">
+      <c r="C918" t="s">
         <v>1816</v>
       </c>
-      <c r="C918" t="s">
+      <c r="D918" t="s">
         <v>1817</v>
-      </c>
-      <c r="D918" t="s">
-        <v>1818</v>
       </c>
       <c r="E918" t="s">
         <v>261</v>
@@ -58246,10 +58177,10 @@
     </row>
     <row r="919">
       <c r="A919" t="s">
+        <v>1814</v>
+      </c>
+      <c r="B919" t="s">
         <v>1815</v>
-      </c>
-      <c r="B919" t="s">
-        <v>1816</v>
       </c>
       <c r="C919" t="s">
         <v>393</v>
@@ -58302,10 +58233,10 @@
     </row>
     <row r="920">
       <c r="A920" t="s">
+        <v>1818</v>
+      </c>
+      <c r="B920" t="s">
         <v>1819</v>
-      </c>
-      <c r="B920" t="s">
-        <v>1820</v>
       </c>
       <c r="C920" t="s">
         <v>1792</v>
@@ -58317,7 +58248,7 @@
         <v>1794</v>
       </c>
       <c r="F920" t="s">
-        <v>1795</v>
+        <v>136</v>
       </c>
       <c r="G920" t="s">
         <v>41</v>
@@ -58358,16 +58289,16 @@
     </row>
     <row r="921">
       <c r="A921" t="s">
+        <v>1818</v>
+      </c>
+      <c r="B921" t="s">
         <v>1819</v>
-      </c>
-      <c r="B921" t="s">
-        <v>1820</v>
       </c>
       <c r="C921" t="s">
         <v>1277</v>
       </c>
       <c r="D921" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="E921" t="s">
         <v>287</v>
@@ -58414,10 +58345,10 @@
     </row>
     <row r="922">
       <c r="A922" t="s">
+        <v>1818</v>
+      </c>
+      <c r="B922" t="s">
         <v>1819</v>
-      </c>
-      <c r="B922" t="s">
-        <v>1820</v>
       </c>
       <c r="C922" t="s">
         <v>242</v>
@@ -58470,10 +58401,10 @@
     </row>
     <row r="923">
       <c r="A923" t="s">
+        <v>1821</v>
+      </c>
+      <c r="B923" t="s">
         <v>1822</v>
-      </c>
-      <c r="B923" t="s">
-        <v>1823</v>
       </c>
       <c r="C923" t="s">
         <v>1792</v>
@@ -58485,7 +58416,7 @@
         <v>1794</v>
       </c>
       <c r="F923" t="s">
-        <v>1795</v>
+        <v>136</v>
       </c>
       <c r="G923" t="s">
         <v>41</v>
@@ -58526,19 +58457,19 @@
     </row>
     <row r="924">
       <c r="A924" t="s">
+        <v>1821</v>
+      </c>
+      <c r="B924" t="s">
         <v>1822</v>
       </c>
-      <c r="B924" t="s">
+      <c r="C924" t="s">
         <v>1823</v>
-      </c>
-      <c r="C924" t="s">
-        <v>1824</v>
       </c>
       <c r="D924" t="s">
         <v>260</v>
       </c>
       <c r="E924" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="F924" t="s">
         <v>251</v>
@@ -58582,10 +58513,10 @@
     </row>
     <row r="925">
       <c r="A925" t="s">
+        <v>1821</v>
+      </c>
+      <c r="B925" t="s">
         <v>1822</v>
-      </c>
-      <c r="B925" t="s">
-        <v>1823</v>
       </c>
       <c r="C925" t="s">
         <v>314</v>
@@ -58594,7 +58525,7 @@
         <v>315</v>
       </c>
       <c r="E925" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
       <c r="F925" t="s">
         <v>251</v>
@@ -58638,10 +58569,10 @@
     </row>
     <row r="926">
       <c r="A926" t="s">
+        <v>1826</v>
+      </c>
+      <c r="B926" t="s">
         <v>1827</v>
-      </c>
-      <c r="B926" t="s">
-        <v>1828</v>
       </c>
       <c r="C926" t="s">
         <v>1792</v>
@@ -58653,7 +58584,7 @@
         <v>1794</v>
       </c>
       <c r="F926" t="s">
-        <v>1795</v>
+        <v>136</v>
       </c>
       <c r="G926" t="s">
         <v>41</v>
@@ -58694,13 +58625,13 @@
     </row>
     <row r="927">
       <c r="A927" t="s">
+        <v>1826</v>
+      </c>
+      <c r="B927" t="s">
         <v>1827</v>
       </c>
-      <c r="B927" t="s">
+      <c r="C927" t="s">
         <v>1828</v>
-      </c>
-      <c r="C927" t="s">
-        <v>1829</v>
       </c>
       <c r="D927" t="s">
         <v>466</v>
@@ -58750,10 +58681,10 @@
     </row>
     <row r="928">
       <c r="A928" t="s">
+        <v>1826</v>
+      </c>
+      <c r="B928" t="s">
         <v>1827</v>
-      </c>
-      <c r="B928" t="s">
-        <v>1828</v>
       </c>
       <c r="C928" t="s">
         <v>1556</v>
@@ -58762,7 +58693,7 @@
         <v>320</v>
       </c>
       <c r="E928" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="F928" t="s">
         <v>209</v>
@@ -58806,10 +58737,10 @@
     </row>
     <row r="929">
       <c r="A929" t="s">
+        <v>1830</v>
+      </c>
+      <c r="B929" t="s">
         <v>1831</v>
-      </c>
-      <c r="B929" t="s">
-        <v>1832</v>
       </c>
       <c r="C929" t="s">
         <v>1792</v>
@@ -58821,7 +58752,7 @@
         <v>1794</v>
       </c>
       <c r="F929" t="s">
-        <v>1795</v>
+        <v>136</v>
       </c>
       <c r="G929" t="s">
         <v>41</v>
@@ -58862,19 +58793,19 @@
     </row>
     <row r="930">
       <c r="A930" t="s">
+        <v>1830</v>
+      </c>
+      <c r="B930" t="s">
         <v>1831</v>
       </c>
-      <c r="B930" t="s">
+      <c r="C930" t="s">
         <v>1832</v>
-      </c>
-      <c r="C930" t="s">
-        <v>1833</v>
       </c>
       <c r="D930" t="s">
         <v>1175</v>
       </c>
       <c r="E930" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="F930" t="s">
         <v>363</v>
@@ -58918,16 +58849,16 @@
     </row>
     <row r="931">
       <c r="A931" t="s">
+        <v>1830</v>
+      </c>
+      <c r="B931" t="s">
         <v>1831</v>
       </c>
-      <c r="B931" t="s">
-        <v>1832</v>
-      </c>
       <c r="C931" t="s">
+        <v>1834</v>
+      </c>
+      <c r="D931" t="s">
         <v>1835</v>
-      </c>
-      <c r="D931" t="s">
-        <v>1836</v>
       </c>
       <c r="E931" t="s">
         <v>69</v>
@@ -58974,10 +58905,10 @@
     </row>
     <row r="932">
       <c r="A932" t="s">
+        <v>1836</v>
+      </c>
+      <c r="B932" t="s">
         <v>1837</v>
-      </c>
-      <c r="B932" t="s">
-        <v>1838</v>
       </c>
       <c r="C932" t="s">
         <v>1792</v>
@@ -58989,7 +58920,7 @@
         <v>1794</v>
       </c>
       <c r="F932" t="s">
-        <v>1795</v>
+        <v>136</v>
       </c>
       <c r="G932" t="s">
         <v>41</v>
@@ -59030,19 +58961,19 @@
     </row>
     <row r="933">
       <c r="A933" t="s">
+        <v>1836</v>
+      </c>
+      <c r="B933" t="s">
         <v>1837</v>
       </c>
-      <c r="B933" t="s">
+      <c r="C933" t="s">
         <v>1838</v>
       </c>
-      <c r="C933" t="s">
+      <c r="D933" t="s">
         <v>1839</v>
       </c>
-      <c r="D933" t="s">
+      <c r="E933" t="s">
         <v>1840</v>
-      </c>
-      <c r="E933" t="s">
-        <v>1841</v>
       </c>
       <c r="F933" t="s">
         <v>60</v>
@@ -59086,19 +59017,19 @@
     </row>
     <row r="934">
       <c r="A934" t="s">
+        <v>1836</v>
+      </c>
+      <c r="B934" t="s">
         <v>1837</v>
       </c>
-      <c r="B934" t="s">
-        <v>1838</v>
-      </c>
       <c r="C934" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="D934" t="s">
         <v>373</v>
       </c>
       <c r="E934" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="F934" t="s">
         <v>84</v>
@@ -59142,10 +59073,10 @@
     </row>
     <row r="935">
       <c r="A935" t="s">
+        <v>1843</v>
+      </c>
+      <c r="B935" t="s">
         <v>1844</v>
-      </c>
-      <c r="B935" t="s">
-        <v>1845</v>
       </c>
       <c r="C935" t="s">
         <v>1792</v>
@@ -59157,7 +59088,7 @@
         <v>1794</v>
       </c>
       <c r="F935" t="s">
-        <v>1795</v>
+        <v>136</v>
       </c>
       <c r="G935" t="s">
         <v>41</v>
@@ -59198,19 +59129,19 @@
     </row>
     <row r="936">
       <c r="A936" t="s">
+        <v>1843</v>
+      </c>
+      <c r="B936" t="s">
         <v>1844</v>
       </c>
-      <c r="B936" t="s">
+      <c r="C936" t="s">
         <v>1845</v>
-      </c>
-      <c r="C936" t="s">
-        <v>1846</v>
       </c>
       <c r="D936" t="s">
         <v>49</v>
       </c>
       <c r="E936" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="F936" t="s">
         <v>64</v>
@@ -59254,16 +59185,16 @@
     </row>
     <row r="937">
       <c r="A937" t="s">
+        <v>1843</v>
+      </c>
+      <c r="B937" t="s">
         <v>1844</v>
       </c>
-      <c r="B937" t="s">
-        <v>1845</v>
-      </c>
       <c r="C937" t="s">
+        <v>1847</v>
+      </c>
+      <c r="D937" t="s">
         <v>1848</v>
-      </c>
-      <c r="D937" t="s">
-        <v>1849</v>
       </c>
       <c r="E937" t="s">
         <v>1214</v>
@@ -59310,13 +59241,13 @@
     </row>
     <row r="938">
       <c r="A938" t="s">
+        <v>1849</v>
+      </c>
+      <c r="B938" t="s">
         <v>1850</v>
       </c>
-      <c r="B938" t="s">
+      <c r="C938" t="s">
         <v>1851</v>
-      </c>
-      <c r="C938" t="s">
-        <v>1852</v>
       </c>
       <c r="D938" t="s">
         <v>588</v>
@@ -59366,13 +59297,13 @@
     </row>
     <row r="939">
       <c r="A939" t="s">
+        <v>1849</v>
+      </c>
+      <c r="B939" t="s">
         <v>1850</v>
       </c>
-      <c r="B939" t="s">
-        <v>1851</v>
-      </c>
       <c r="C939" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="D939" t="s">
         <v>408</v>
@@ -59422,19 +59353,19 @@
     </row>
     <row r="940">
       <c r="A940" t="s">
+        <v>1849</v>
+      </c>
+      <c r="B940" t="s">
         <v>1850</v>
       </c>
-      <c r="B940" t="s">
-        <v>1851</v>
-      </c>
       <c r="C940" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="D940" t="s">
         <v>466</v>
       </c>
       <c r="E940" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="F940" t="s">
         <v>70</v>
@@ -59478,13 +59409,13 @@
     </row>
     <row r="941">
       <c r="A941" t="s">
+        <v>1855</v>
+      </c>
+      <c r="B941" t="s">
         <v>1856</v>
       </c>
-      <c r="B941" t="s">
-        <v>1857</v>
-      </c>
       <c r="C941" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="D941" t="s">
         <v>588</v>
@@ -59534,13 +59465,13 @@
     </row>
     <row r="942">
       <c r="A942" t="s">
+        <v>1855</v>
+      </c>
+      <c r="B942" t="s">
         <v>1856</v>
       </c>
-      <c r="B942" t="s">
-        <v>1857</v>
-      </c>
       <c r="C942" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="D942" t="s">
         <v>408</v>
@@ -59590,19 +59521,19 @@
     </row>
     <row r="943">
       <c r="A943" t="s">
+        <v>1855</v>
+      </c>
+      <c r="B943" t="s">
         <v>1856</v>
       </c>
-      <c r="B943" t="s">
-        <v>1857</v>
-      </c>
       <c r="C943" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="D943" t="s">
         <v>466</v>
       </c>
       <c r="E943" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="F943" t="s">
         <v>70</v>
@@ -59646,13 +59577,13 @@
     </row>
     <row r="944">
       <c r="A944" t="s">
+        <v>1857</v>
+      </c>
+      <c r="B944" t="s">
         <v>1858</v>
       </c>
-      <c r="B944" t="s">
-        <v>1859</v>
-      </c>
       <c r="C944" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="D944" t="s">
         <v>588</v>
@@ -59702,13 +59633,13 @@
     </row>
     <row r="945">
       <c r="A945" t="s">
+        <v>1857</v>
+      </c>
+      <c r="B945" t="s">
         <v>1858</v>
       </c>
-      <c r="B945" t="s">
-        <v>1859</v>
-      </c>
       <c r="C945" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="D945" t="s">
         <v>408</v>
@@ -59758,19 +59689,19 @@
     </row>
     <row r="946">
       <c r="A946" t="s">
+        <v>1857</v>
+      </c>
+      <c r="B946" t="s">
         <v>1858</v>
       </c>
-      <c r="B946" t="s">
-        <v>1859</v>
-      </c>
       <c r="C946" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="D946" t="s">
         <v>466</v>
       </c>
       <c r="E946" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="F946" t="s">
         <v>70</v>
@@ -59814,13 +59745,13 @@
     </row>
     <row r="947">
       <c r="A947" t="s">
+        <v>1859</v>
+      </c>
+      <c r="B947" t="s">
         <v>1860</v>
       </c>
-      <c r="B947" t="s">
-        <v>1861</v>
-      </c>
       <c r="C947" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="D947" t="s">
         <v>588</v>
@@ -59870,13 +59801,13 @@
     </row>
     <row r="948">
       <c r="A948" t="s">
+        <v>1859</v>
+      </c>
+      <c r="B948" t="s">
         <v>1860</v>
       </c>
-      <c r="B948" t="s">
-        <v>1861</v>
-      </c>
       <c r="C948" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="D948" t="s">
         <v>408</v>
@@ -59926,19 +59857,19 @@
     </row>
     <row r="949">
       <c r="A949" t="s">
+        <v>1859</v>
+      </c>
+      <c r="B949" t="s">
         <v>1860</v>
       </c>
-      <c r="B949" t="s">
-        <v>1861</v>
-      </c>
       <c r="C949" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="D949" t="s">
         <v>466</v>
       </c>
       <c r="E949" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="F949" t="s">
         <v>70</v>
@@ -59982,13 +59913,13 @@
     </row>
     <row r="950">
       <c r="A950" t="s">
+        <v>1861</v>
+      </c>
+      <c r="B950" t="s">
         <v>1862</v>
       </c>
-      <c r="B950" t="s">
-        <v>1863</v>
-      </c>
       <c r="C950" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="D950" t="s">
         <v>588</v>
@@ -60038,13 +59969,13 @@
     </row>
     <row r="951">
       <c r="A951" t="s">
+        <v>1861</v>
+      </c>
+      <c r="B951" t="s">
         <v>1862</v>
       </c>
-      <c r="B951" t="s">
-        <v>1863</v>
-      </c>
       <c r="C951" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="D951" t="s">
         <v>408</v>
@@ -60094,19 +60025,19 @@
     </row>
     <row r="952">
       <c r="A952" t="s">
+        <v>1861</v>
+      </c>
+      <c r="B952" t="s">
         <v>1862</v>
       </c>
-      <c r="B952" t="s">
-        <v>1863</v>
-      </c>
       <c r="C952" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="D952" t="s">
         <v>466</v>
       </c>
       <c r="E952" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="F952" t="s">
         <v>70</v>
@@ -60150,13 +60081,13 @@
     </row>
     <row r="953">
       <c r="A953" t="s">
+        <v>1863</v>
+      </c>
+      <c r="B953" t="s">
         <v>1864</v>
       </c>
-      <c r="B953" t="s">
-        <v>1865</v>
-      </c>
       <c r="C953" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="D953" t="s">
         <v>588</v>
@@ -60206,13 +60137,13 @@
     </row>
     <row r="954">
       <c r="A954" t="s">
+        <v>1863</v>
+      </c>
+      <c r="B954" t="s">
         <v>1864</v>
       </c>
-      <c r="B954" t="s">
-        <v>1865</v>
-      </c>
       <c r="C954" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="D954" t="s">
         <v>408</v>
@@ -60262,19 +60193,19 @@
     </row>
     <row r="955">
       <c r="A955" t="s">
+        <v>1863</v>
+      </c>
+      <c r="B955" t="s">
         <v>1864</v>
       </c>
-      <c r="B955" t="s">
-        <v>1865</v>
-      </c>
       <c r="C955" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="D955" t="s">
         <v>466</v>
       </c>
       <c r="E955" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="F955" t="s">
         <v>70</v>
@@ -60318,16 +60249,16 @@
     </row>
     <row r="956">
       <c r="A956" t="s">
+        <v>1865</v>
+      </c>
+      <c r="B956" t="s">
         <v>1866</v>
       </c>
-      <c r="B956" t="s">
+      <c r="C956" t="s">
         <v>1867</v>
       </c>
-      <c r="C956" t="s">
+      <c r="D956" t="s">
         <v>1868</v>
-      </c>
-      <c r="D956" t="s">
-        <v>1869</v>
       </c>
       <c r="E956" t="s">
         <v>89</v>
@@ -60374,13 +60305,13 @@
     </row>
     <row r="957">
       <c r="A957" t="s">
+        <v>1865</v>
+      </c>
+      <c r="B957" t="s">
         <v>1866</v>
       </c>
-      <c r="B957" t="s">
-        <v>1867</v>
-      </c>
       <c r="C957" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="D957" t="s">
         <v>1278</v>
@@ -60430,13 +60361,13 @@
     </row>
     <row r="958">
       <c r="A958" t="s">
+        <v>1865</v>
+      </c>
+      <c r="B958" t="s">
         <v>1866</v>
       </c>
-      <c r="B958" t="s">
-        <v>1867</v>
-      </c>
       <c r="C958" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="D958" t="s">
         <v>408</v>
@@ -60486,13 +60417,13 @@
     </row>
     <row r="959">
       <c r="A959" t="s">
+        <v>1870</v>
+      </c>
+      <c r="B959" t="s">
         <v>1871</v>
       </c>
-      <c r="B959" t="s">
+      <c r="C959" t="s">
         <v>1872</v>
-      </c>
-      <c r="C959" t="s">
-        <v>1873</v>
       </c>
       <c r="D959" t="s">
         <v>243</v>
@@ -60542,19 +60473,19 @@
     </row>
     <row r="960">
       <c r="A960" t="s">
+        <v>1870</v>
+      </c>
+      <c r="B960" t="s">
         <v>1871</v>
       </c>
-      <c r="B960" t="s">
-        <v>1872</v>
-      </c>
       <c r="C960" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="D960" t="s">
         <v>373</v>
       </c>
       <c r="E960" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="F960" t="s">
         <v>60</v>
@@ -60598,19 +60529,19 @@
     </row>
     <row r="961">
       <c r="A961" t="s">
+        <v>1870</v>
+      </c>
+      <c r="B961" t="s">
         <v>1871</v>
       </c>
-      <c r="B961" t="s">
-        <v>1872</v>
-      </c>
       <c r="C961" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="D961" t="s">
         <v>466</v>
       </c>
       <c r="E961" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="F961" t="s">
         <v>70</v>
@@ -60654,13 +60585,13 @@
     </row>
     <row r="962">
       <c r="A962" t="s">
+        <v>1875</v>
+      </c>
+      <c r="B962" t="s">
         <v>1876</v>
       </c>
-      <c r="B962" t="s">
-        <v>1877</v>
-      </c>
       <c r="C962" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="D962" t="s">
         <v>588</v>
@@ -60710,16 +60641,16 @@
     </row>
     <row r="963">
       <c r="A963" t="s">
+        <v>1875</v>
+      </c>
+      <c r="B963" t="s">
         <v>1876</v>
       </c>
-      <c r="B963" t="s">
+      <c r="C963" t="s">
         <v>1877</v>
       </c>
-      <c r="C963" t="s">
+      <c r="D963" t="s">
         <v>1878</v>
-      </c>
-      <c r="D963" t="s">
-        <v>1879</v>
       </c>
       <c r="E963" t="s">
         <v>1651</v>
@@ -60766,13 +60697,13 @@
     </row>
     <row r="964">
       <c r="A964" t="s">
+        <v>1875</v>
+      </c>
+      <c r="B964" t="s">
         <v>1876</v>
       </c>
-      <c r="B964" t="s">
-        <v>1877</v>
-      </c>
       <c r="C964" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="D964" t="s">
         <v>184</v>
@@ -60822,13 +60753,13 @@
     </row>
     <row r="965">
       <c r="A965" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B965" t="s">
         <v>1881</v>
       </c>
-      <c r="B965" t="s">
+      <c r="C965" t="s">
         <v>1882</v>
-      </c>
-      <c r="C965" t="s">
-        <v>1883</v>
       </c>
       <c r="D965" t="s">
         <v>928</v>
@@ -60878,13 +60809,13 @@
     </row>
     <row r="966">
       <c r="A966" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B966" t="s">
         <v>1881</v>
       </c>
-      <c r="B966" t="s">
-        <v>1882</v>
-      </c>
       <c r="C966" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="D966" t="s">
         <v>1435</v>
@@ -60934,19 +60865,19 @@
     </row>
     <row r="967">
       <c r="A967" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B967" t="s">
         <v>1881</v>
       </c>
-      <c r="B967" t="s">
-        <v>1882</v>
-      </c>
       <c r="C967" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="D967" t="s">
         <v>466</v>
       </c>
       <c r="E967" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="F967" t="s">
         <v>70</v>
@@ -60990,13 +60921,13 @@
     </row>
     <row r="968">
       <c r="A968" t="s">
+        <v>1884</v>
+      </c>
+      <c r="B968" t="s">
         <v>1885</v>
       </c>
-      <c r="B968" t="s">
-        <v>1886</v>
-      </c>
       <c r="C968" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="D968" t="s">
         <v>1278</v>
@@ -61046,19 +60977,19 @@
     </row>
     <row r="969">
       <c r="A969" t="s">
+        <v>1884</v>
+      </c>
+      <c r="B969" t="s">
         <v>1885</v>
       </c>
-      <c r="B969" t="s">
+      <c r="C969" t="s">
         <v>1886</v>
       </c>
-      <c r="C969" t="s">
+      <c r="D969" t="s">
         <v>1887</v>
       </c>
-      <c r="D969" t="s">
+      <c r="E969" t="s">
         <v>1888</v>
-      </c>
-      <c r="E969" t="s">
-        <v>1889</v>
       </c>
       <c r="F969" t="s">
         <v>60</v>
@@ -61102,16 +61033,16 @@
     </row>
     <row r="970">
       <c r="A970" t="s">
+        <v>1884</v>
+      </c>
+      <c r="B970" t="s">
         <v>1885</v>
-      </c>
-      <c r="B970" t="s">
-        <v>1886</v>
       </c>
       <c r="C970" t="s">
         <v>308</v>
       </c>
       <c r="D970" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="E970" t="s">
         <v>1316</v>
@@ -61158,13 +61089,13 @@
     </row>
     <row r="971">
       <c r="A971" t="s">
+        <v>1890</v>
+      </c>
+      <c r="B971" t="s">
         <v>1891</v>
       </c>
-      <c r="B971" t="s">
+      <c r="C971" t="s">
         <v>1892</v>
-      </c>
-      <c r="C971" t="s">
-        <v>1893</v>
       </c>
       <c r="D971" t="s">
         <v>1029</v>
@@ -61214,16 +61145,16 @@
     </row>
     <row r="972">
       <c r="A972" t="s">
+        <v>1890</v>
+      </c>
+      <c r="B972" t="s">
         <v>1891</v>
       </c>
-      <c r="B972" t="s">
-        <v>1892</v>
-      </c>
       <c r="C972" t="s">
+        <v>1893</v>
+      </c>
+      <c r="D972" t="s">
         <v>1894</v>
-      </c>
-      <c r="D972" t="s">
-        <v>1895</v>
       </c>
       <c r="E972" t="s">
         <v>63</v>
@@ -61270,19 +61201,19 @@
     </row>
     <row r="973">
       <c r="A973" t="s">
+        <v>1890</v>
+      </c>
+      <c r="B973" t="s">
         <v>1891</v>
       </c>
-      <c r="B973" t="s">
-        <v>1892</v>
-      </c>
       <c r="C973" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="D973" t="s">
         <v>373</v>
       </c>
       <c r="E973" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="F973" t="s">
         <v>60</v>
@@ -61326,13 +61257,13 @@
     </row>
     <row r="974">
       <c r="A974" t="s">
+        <v>1895</v>
+      </c>
+      <c r="B974" t="s">
         <v>1896</v>
       </c>
-      <c r="B974" t="s">
+      <c r="C974" t="s">
         <v>1897</v>
-      </c>
-      <c r="C974" t="s">
-        <v>1898</v>
       </c>
       <c r="D974" t="s">
         <v>43</v>
@@ -61382,13 +61313,13 @@
     </row>
     <row r="975">
       <c r="A975" t="s">
+        <v>1895</v>
+      </c>
+      <c r="B975" t="s">
         <v>1896</v>
       </c>
-      <c r="B975" t="s">
-        <v>1897</v>
-      </c>
       <c r="C975" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="D975" t="s">
         <v>184</v>
@@ -61438,16 +61369,16 @@
     </row>
     <row r="976">
       <c r="A976" t="s">
+        <v>1895</v>
+      </c>
+      <c r="B976" t="s">
         <v>1896</v>
-      </c>
-      <c r="B976" t="s">
-        <v>1897</v>
       </c>
       <c r="C976" t="s">
         <v>1520</v>
       </c>
       <c r="D976" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="E976" t="s">
         <v>324</v>
@@ -61494,19 +61425,19 @@
     </row>
     <row r="977">
       <c r="A977" t="s">
+        <v>1899</v>
+      </c>
+      <c r="B977" t="s">
         <v>1900</v>
       </c>
-      <c r="B977" t="s">
+      <c r="C977" t="s">
         <v>1901</v>
-      </c>
-      <c r="C977" t="s">
-        <v>1902</v>
       </c>
       <c r="D977" t="s">
         <v>1085</v>
       </c>
       <c r="E977" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
       <c r="F977" t="s">
         <v>28</v>
@@ -61550,13 +61481,13 @@
     </row>
     <row r="978">
       <c r="A978" t="s">
+        <v>1899</v>
+      </c>
+      <c r="B978" t="s">
         <v>1900</v>
       </c>
-      <c r="B978" t="s">
-        <v>1901</v>
-      </c>
       <c r="C978" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="D978" t="s">
         <v>408</v>
@@ -61606,19 +61537,19 @@
     </row>
     <row r="979">
       <c r="A979" t="s">
+        <v>1899</v>
+      </c>
+      <c r="B979" t="s">
         <v>1900</v>
       </c>
-      <c r="B979" t="s">
-        <v>1901</v>
-      </c>
       <c r="C979" t="s">
+        <v>1903</v>
+      </c>
+      <c r="D979" t="s">
         <v>1904</v>
       </c>
-      <c r="D979" t="s">
+      <c r="E979" t="s">
         <v>1905</v>
-      </c>
-      <c r="E979" t="s">
-        <v>1906</v>
       </c>
       <c r="F979" t="s">
         <v>45</v>
@@ -61662,10 +61593,10 @@
     </row>
     <row r="980">
       <c r="A980" t="s">
+        <v>1906</v>
+      </c>
+      <c r="B980" t="s">
         <v>1907</v>
-      </c>
-      <c r="B980" t="s">
-        <v>1908</v>
       </c>
       <c r="C980" t="s">
         <v>198</v>
@@ -61718,13 +61649,13 @@
     </row>
     <row r="981">
       <c r="A981" t="s">
+        <v>1906</v>
+      </c>
+      <c r="B981" t="s">
         <v>1907</v>
       </c>
-      <c r="B981" t="s">
+      <c r="C981" t="s">
         <v>1908</v>
-      </c>
-      <c r="C981" t="s">
-        <v>1909</v>
       </c>
       <c r="D981" t="s">
         <v>1175</v>
@@ -61774,16 +61705,16 @@
     </row>
     <row r="982">
       <c r="A982" t="s">
+        <v>1906</v>
+      </c>
+      <c r="B982" t="s">
         <v>1907</v>
       </c>
-      <c r="B982" t="s">
-        <v>1908</v>
-      </c>
       <c r="C982" t="s">
+        <v>1877</v>
+      </c>
+      <c r="D982" t="s">
         <v>1878</v>
-      </c>
-      <c r="D982" t="s">
-        <v>1879</v>
       </c>
       <c r="E982" t="s">
         <v>1651</v>
@@ -61830,16 +61761,16 @@
     </row>
     <row r="983">
       <c r="A983" t="s">
+        <v>1909</v>
+      </c>
+      <c r="B983" t="s">
         <v>1910</v>
       </c>
-      <c r="B983" t="s">
-        <v>1911</v>
-      </c>
       <c r="C983" t="s">
+        <v>1893</v>
+      </c>
+      <c r="D983" t="s">
         <v>1894</v>
-      </c>
-      <c r="D983" t="s">
-        <v>1895</v>
       </c>
       <c r="E983" t="s">
         <v>63</v>
@@ -61886,19 +61817,19 @@
     </row>
     <row r="984">
       <c r="A984" t="s">
+        <v>1909</v>
+      </c>
+      <c r="B984" t="s">
         <v>1910</v>
       </c>
-      <c r="B984" t="s">
+      <c r="C984" t="s">
         <v>1911</v>
-      </c>
-      <c r="C984" t="s">
-        <v>1912</v>
       </c>
       <c r="D984" t="s">
         <v>1528</v>
       </c>
       <c r="E984" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="F984" t="s">
         <v>70</v>
@@ -61942,16 +61873,16 @@
     </row>
     <row r="985">
       <c r="A985" t="s">
+        <v>1909</v>
+      </c>
+      <c r="B985" t="s">
         <v>1910</v>
       </c>
-      <c r="B985" t="s">
-        <v>1911</v>
-      </c>
       <c r="C985" t="s">
+        <v>1913</v>
+      </c>
+      <c r="D985" t="s">
         <v>1914</v>
-      </c>
-      <c r="D985" t="s">
-        <v>1915</v>
       </c>
       <c r="E985" t="s">
         <v>1259</v>
@@ -61998,16 +61929,16 @@
     </row>
     <row r="986">
       <c r="A986" t="s">
+        <v>1915</v>
+      </c>
+      <c r="B986" t="s">
         <v>1916</v>
       </c>
-      <c r="B986" t="s">
-        <v>1917</v>
-      </c>
       <c r="C986" t="s">
+        <v>1893</v>
+      </c>
+      <c r="D986" t="s">
         <v>1894</v>
-      </c>
-      <c r="D986" t="s">
-        <v>1895</v>
       </c>
       <c r="E986" t="s">
         <v>63</v>
@@ -62054,19 +61985,19 @@
     </row>
     <row r="987">
       <c r="A987" t="s">
+        <v>1915</v>
+      </c>
+      <c r="B987" t="s">
         <v>1916</v>
       </c>
-      <c r="B987" t="s">
-        <v>1917</v>
-      </c>
       <c r="C987" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="D987" t="s">
         <v>1528</v>
       </c>
       <c r="E987" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="F987" t="s">
         <v>70</v>
@@ -62110,16 +62041,16 @@
     </row>
     <row r="988">
       <c r="A988" t="s">
+        <v>1915</v>
+      </c>
+      <c r="B988" t="s">
         <v>1916</v>
       </c>
-      <c r="B988" t="s">
-        <v>1917</v>
-      </c>
       <c r="C988" t="s">
+        <v>1913</v>
+      </c>
+      <c r="D988" t="s">
         <v>1914</v>
-      </c>
-      <c r="D988" t="s">
-        <v>1915</v>
       </c>
       <c r="E988" t="s">
         <v>1259</v>
@@ -62166,16 +62097,16 @@
     </row>
     <row r="989">
       <c r="A989" t="s">
+        <v>1917</v>
+      </c>
+      <c r="B989" t="s">
         <v>1918</v>
       </c>
-      <c r="B989" t="s">
+      <c r="C989" t="s">
         <v>1919</v>
       </c>
-      <c r="C989" t="s">
+      <c r="D989" t="s">
         <v>1920</v>
-      </c>
-      <c r="D989" t="s">
-        <v>1921</v>
       </c>
       <c r="E989" t="s">
         <v>109</v>
@@ -62222,16 +62153,16 @@
     </row>
     <row r="990">
       <c r="A990" t="s">
+        <v>1917</v>
+      </c>
+      <c r="B990" t="s">
         <v>1918</v>
       </c>
-      <c r="B990" t="s">
-        <v>1919</v>
-      </c>
       <c r="C990" t="s">
+        <v>1921</v>
+      </c>
+      <c r="D990" t="s">
         <v>1922</v>
-      </c>
-      <c r="D990" t="s">
-        <v>1923</v>
       </c>
       <c r="E990" t="s">
         <v>950</v>
@@ -62278,16 +62209,16 @@
     </row>
     <row r="991">
       <c r="A991" t="s">
+        <v>1917</v>
+      </c>
+      <c r="B991" t="s">
         <v>1918</v>
       </c>
-      <c r="B991" t="s">
-        <v>1919</v>
-      </c>
       <c r="C991" t="s">
+        <v>1893</v>
+      </c>
+      <c r="D991" t="s">
         <v>1894</v>
-      </c>
-      <c r="D991" t="s">
-        <v>1895</v>
       </c>
       <c r="E991" t="s">
         <v>63</v>
@@ -62334,13 +62265,13 @@
     </row>
     <row r="992">
       <c r="A992" t="s">
+        <v>1923</v>
+      </c>
+      <c r="B992" t="s">
         <v>1924</v>
       </c>
-      <c r="B992" t="s">
+      <c r="C992" t="s">
         <v>1925</v>
-      </c>
-      <c r="C992" t="s">
-        <v>1926</v>
       </c>
       <c r="D992" t="s">
         <v>1002</v>
@@ -62390,13 +62321,13 @@
     </row>
     <row r="993">
       <c r="A993" t="s">
+        <v>1923</v>
+      </c>
+      <c r="B993" t="s">
         <v>1924</v>
       </c>
-      <c r="B993" t="s">
-        <v>1925</v>
-      </c>
       <c r="C993" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="D993" t="s">
         <v>925</v>
@@ -62446,19 +62377,19 @@
     </row>
     <row r="994">
       <c r="A994" t="s">
+        <v>1923</v>
+      </c>
+      <c r="B994" t="s">
         <v>1924</v>
       </c>
-      <c r="B994" t="s">
-        <v>1925</v>
-      </c>
       <c r="C994" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="D994" t="s">
         <v>1528</v>
       </c>
       <c r="E994" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="F994" t="s">
         <v>70</v>
@@ -62502,19 +62433,19 @@
     </row>
     <row r="995">
       <c r="A995" t="s">
+        <v>1927</v>
+      </c>
+      <c r="B995" t="s">
         <v>1928</v>
       </c>
-      <c r="B995" t="s">
+      <c r="C995" t="s">
         <v>1929</v>
-      </c>
-      <c r="C995" t="s">
-        <v>1930</v>
       </c>
       <c r="D995" t="s">
         <v>701</v>
       </c>
       <c r="E995" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
       <c r="F995" t="s">
         <v>154</v>
@@ -62558,10 +62489,10 @@
     </row>
     <row r="996">
       <c r="A996" t="s">
+        <v>1927</v>
+      </c>
+      <c r="B996" t="s">
         <v>1928</v>
-      </c>
-      <c r="B996" t="s">
-        <v>1929</v>
       </c>
       <c r="C996" t="s">
         <v>1556</v>
@@ -62614,16 +62545,16 @@
     </row>
     <row r="997">
       <c r="A997" t="s">
+        <v>1927</v>
+      </c>
+      <c r="B997" t="s">
         <v>1928</v>
       </c>
-      <c r="B997" t="s">
-        <v>1929</v>
-      </c>
       <c r="C997" t="s">
+        <v>1913</v>
+      </c>
+      <c r="D997" t="s">
         <v>1914</v>
-      </c>
-      <c r="D997" t="s">
-        <v>1915</v>
       </c>
       <c r="E997" t="s">
         <v>1259</v>
@@ -62670,19 +62601,19 @@
     </row>
     <row r="998">
       <c r="A998" t="s">
+        <v>1931</v>
+      </c>
+      <c r="B998" t="s">
         <v>1932</v>
       </c>
-      <c r="B998" t="s">
+      <c r="C998" t="s">
         <v>1933</v>
-      </c>
-      <c r="C998" t="s">
-        <v>1934</v>
       </c>
       <c r="D998" t="s">
         <v>185</v>
       </c>
       <c r="E998" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="F998" t="s">
         <v>70</v>
@@ -62726,13 +62657,13 @@
     </row>
     <row r="999">
       <c r="A999" t="s">
+        <v>1931</v>
+      </c>
+      <c r="B999" t="s">
         <v>1932</v>
       </c>
-      <c r="B999" t="s">
-        <v>1933</v>
-      </c>
       <c r="C999" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="D999" t="s">
         <v>1435</v>
@@ -62782,16 +62713,16 @@
     </row>
     <row r="1000">
       <c r="A1000" t="s">
+        <v>1931</v>
+      </c>
+      <c r="B1000" t="s">
         <v>1932</v>
       </c>
-      <c r="B1000" t="s">
-        <v>1933</v>
-      </c>
       <c r="C1000" t="s">
+        <v>1935</v>
+      </c>
+      <c r="D1000" t="s">
         <v>1936</v>
-      </c>
-      <c r="D1000" t="s">
-        <v>1937</v>
       </c>
       <c r="E1000" t="s">
         <v>678</v>
@@ -62838,19 +62769,19 @@
     </row>
     <row r="1001">
       <c r="A1001" t="s">
+        <v>1937</v>
+      </c>
+      <c r="B1001" t="s">
         <v>1938</v>
       </c>
-      <c r="B1001" t="s">
-        <v>1939</v>
-      </c>
       <c r="C1001" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="D1001" t="s">
         <v>185</v>
       </c>
       <c r="E1001" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="F1001" t="s">
         <v>70</v>
@@ -62894,13 +62825,13 @@
     </row>
     <row r="1002">
       <c r="A1002" t="s">
+        <v>1937</v>
+      </c>
+      <c r="B1002" t="s">
         <v>1938</v>
       </c>
-      <c r="B1002" t="s">
-        <v>1939</v>
-      </c>
       <c r="C1002" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="D1002" t="s">
         <v>1435</v>
@@ -62950,16 +62881,16 @@
     </row>
     <row r="1003">
       <c r="A1003" t="s">
+        <v>1937</v>
+      </c>
+      <c r="B1003" t="s">
         <v>1938</v>
       </c>
-      <c r="B1003" t="s">
-        <v>1939</v>
-      </c>
       <c r="C1003" t="s">
+        <v>1935</v>
+      </c>
+      <c r="D1003" t="s">
         <v>1936</v>
-      </c>
-      <c r="D1003" t="s">
-        <v>1937</v>
       </c>
       <c r="E1003" t="s">
         <v>678</v>
@@ -63006,19 +62937,19 @@
     </row>
     <row r="1004">
       <c r="A1004" t="s">
+        <v>1939</v>
+      </c>
+      <c r="B1004" t="s">
         <v>1940</v>
       </c>
-      <c r="B1004" t="s">
-        <v>1941</v>
-      </c>
       <c r="C1004" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="D1004" t="s">
         <v>185</v>
       </c>
       <c r="E1004" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="F1004" t="s">
         <v>70</v>
@@ -63062,16 +62993,16 @@
     </row>
     <row r="1005">
       <c r="A1005" t="s">
+        <v>1939</v>
+      </c>
+      <c r="B1005" t="s">
         <v>1940</v>
       </c>
-      <c r="B1005" t="s">
+      <c r="C1005" t="s">
         <v>1941</v>
       </c>
-      <c r="C1005" t="s">
+      <c r="D1005" t="s">
         <v>1942</v>
-      </c>
-      <c r="D1005" t="s">
-        <v>1943</v>
       </c>
       <c r="E1005" t="s">
         <v>83</v>
@@ -63118,19 +63049,19 @@
     </row>
     <row r="1006">
       <c r="A1006" t="s">
+        <v>1939</v>
+      </c>
+      <c r="B1006" t="s">
         <v>1940</v>
       </c>
-      <c r="B1006" t="s">
-        <v>1941</v>
-      </c>
       <c r="C1006" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="D1006" t="s">
         <v>388</v>
       </c>
       <c r="E1006" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="F1006" t="s">
         <v>118</v>
@@ -63174,13 +63105,13 @@
     </row>
     <row r="1007">
       <c r="A1007" t="s">
+        <v>1945</v>
+      </c>
+      <c r="B1007" t="s">
         <v>1946</v>
       </c>
-      <c r="B1007" t="s">
+      <c r="C1007" t="s">
         <v>1947</v>
-      </c>
-      <c r="C1007" t="s">
-        <v>1948</v>
       </c>
       <c r="D1007" t="s">
         <v>1090</v>
@@ -63230,19 +63161,19 @@
     </row>
     <row r="1008">
       <c r="A1008" t="s">
+        <v>1945</v>
+      </c>
+      <c r="B1008" t="s">
         <v>1946</v>
       </c>
-      <c r="B1008" t="s">
-        <v>1947</v>
-      </c>
       <c r="C1008" t="s">
+        <v>1948</v>
+      </c>
+      <c r="D1008" t="s">
         <v>1949</v>
       </c>
-      <c r="D1008" t="s">
+      <c r="E1008" t="s">
         <v>1950</v>
-      </c>
-      <c r="E1008" t="s">
-        <v>1951</v>
       </c>
       <c r="F1008" t="s">
         <v>23</v>
@@ -63286,16 +63217,16 @@
     </row>
     <row r="1009">
       <c r="A1009" t="s">
+        <v>1945</v>
+      </c>
+      <c r="B1009" t="s">
         <v>1946</v>
       </c>
-      <c r="B1009" t="s">
-        <v>1947</v>
-      </c>
       <c r="C1009" t="s">
+        <v>1935</v>
+      </c>
+      <c r="D1009" t="s">
         <v>1936</v>
-      </c>
-      <c r="D1009" t="s">
-        <v>1937</v>
       </c>
       <c r="E1009" t="s">
         <v>678</v>
@@ -63342,16 +63273,16 @@
     </row>
     <row r="1010">
       <c r="A1010" t="s">
+        <v>1951</v>
+      </c>
+      <c r="B1010" t="s">
         <v>1952</v>
       </c>
-      <c r="B1010" t="s">
+      <c r="C1010" t="s">
         <v>1953</v>
       </c>
-      <c r="C1010" t="s">
+      <c r="D1010" t="s">
         <v>1954</v>
-      </c>
-      <c r="D1010" t="s">
-        <v>1955</v>
       </c>
       <c r="E1010" t="s">
         <v>118</v>
@@ -63398,13 +63329,13 @@
     </row>
     <row r="1011">
       <c r="A1011" t="s">
+        <v>1951</v>
+      </c>
+      <c r="B1011" t="s">
         <v>1952</v>
       </c>
-      <c r="B1011" t="s">
-        <v>1953</v>
-      </c>
       <c r="C1011" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="D1011" t="s">
         <v>662</v>
@@ -63454,13 +63385,13 @@
     </row>
     <row r="1012">
       <c r="A1012" t="s">
+        <v>1951</v>
+      </c>
+      <c r="B1012" t="s">
         <v>1952</v>
       </c>
-      <c r="B1012" t="s">
-        <v>1953</v>
-      </c>
       <c r="C1012" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="D1012" t="s">
         <v>1435</v>
@@ -63510,10 +63441,10 @@
     </row>
     <row r="1013">
       <c r="A1013" t="s">
+        <v>1956</v>
+      </c>
+      <c r="B1013" t="s">
         <v>1957</v>
-      </c>
-      <c r="B1013" t="s">
-        <v>1958</v>
       </c>
       <c r="C1013" t="s">
         <v>1792</v>
@@ -63525,7 +63456,7 @@
         <v>1794</v>
       </c>
       <c r="F1013" t="s">
-        <v>1795</v>
+        <v>136</v>
       </c>
       <c r="G1013" t="s">
         <v>41</v>
@@ -63566,22 +63497,22 @@
     </row>
     <row r="1014">
       <c r="A1014" t="s">
+        <v>1956</v>
+      </c>
+      <c r="B1014" t="s">
         <v>1957</v>
       </c>
-      <c r="B1014" t="s">
+      <c r="C1014" t="s">
         <v>1958</v>
       </c>
-      <c r="C1014" t="s">
+      <c r="D1014" t="s">
         <v>1959</v>
       </c>
-      <c r="D1014" t="s">
+      <c r="E1014" t="s">
         <v>1960</v>
       </c>
-      <c r="E1014" t="s">
-        <v>1961</v>
-      </c>
       <c r="F1014" t="s">
-        <v>1962</v>
+        <v>70</v>
       </c>
       <c r="G1014" t="s">
         <v>24</v>
@@ -63622,22 +63553,22 @@
     </row>
     <row r="1015">
       <c r="A1015" t="s">
+        <v>1956</v>
+      </c>
+      <c r="B1015" t="s">
         <v>1957</v>
       </c>
-      <c r="B1015" t="s">
-        <v>1958</v>
-      </c>
       <c r="C1015" t="s">
+        <v>1961</v>
+      </c>
+      <c r="D1015" t="s">
+        <v>1962</v>
+      </c>
+      <c r="E1015" t="s">
         <v>1963</v>
       </c>
-      <c r="D1015" t="s">
-        <v>1964</v>
-      </c>
-      <c r="E1015" t="s">
-        <v>1965</v>
-      </c>
       <c r="F1015" t="s">
-        <v>1966</v>
+        <v>90</v>
       </c>
       <c r="G1015" t="s">
         <v>24</v>
@@ -63678,10 +63609,10 @@
     </row>
     <row r="1016">
       <c r="A1016" t="s">
-        <v>1967</v>
+        <v>1964</v>
       </c>
       <c r="B1016" t="s">
-        <v>1968</v>
+        <v>1965</v>
       </c>
       <c r="C1016" t="s">
         <v>1792</v>
@@ -63693,7 +63624,7 @@
         <v>1794</v>
       </c>
       <c r="F1016" t="s">
-        <v>1795</v>
+        <v>136</v>
       </c>
       <c r="G1016" t="s">
         <v>41</v>
@@ -63734,22 +63665,22 @@
     </row>
     <row r="1017">
       <c r="A1017" t="s">
+        <v>1964</v>
+      </c>
+      <c r="B1017" t="s">
+        <v>1965</v>
+      </c>
+      <c r="C1017" t="s">
+        <v>1966</v>
+      </c>
+      <c r="D1017" t="s">
         <v>1967</v>
       </c>
-      <c r="B1017" t="s">
+      <c r="E1017" t="s">
         <v>1968</v>
       </c>
-      <c r="C1017" t="s">
-        <v>1969</v>
-      </c>
-      <c r="D1017" t="s">
-        <v>1970</v>
-      </c>
-      <c r="E1017" t="s">
-        <v>1971</v>
-      </c>
       <c r="F1017" t="s">
-        <v>1972</v>
+        <v>209</v>
       </c>
       <c r="G1017" t="s">
         <v>24</v>
@@ -63790,22 +63721,22 @@
     </row>
     <row r="1018">
       <c r="A1018" t="s">
-        <v>1967</v>
+        <v>1964</v>
       </c>
       <c r="B1018" t="s">
-        <v>1968</v>
+        <v>1965</v>
       </c>
       <c r="C1018" t="s">
-        <v>1973</v>
+        <v>1969</v>
       </c>
       <c r="D1018" t="s">
-        <v>1974</v>
+        <v>1970</v>
       </c>
       <c r="E1018" t="s">
-        <v>1975</v>
+        <v>1971</v>
       </c>
       <c r="F1018" t="s">
-        <v>1976</v>
+        <v>118</v>
       </c>
       <c r="G1018" t="s">
         <v>24</v>
@@ -63846,10 +63777,10 @@
     </row>
     <row r="1019">
       <c r="A1019" t="s">
-        <v>1977</v>
+        <v>1972</v>
       </c>
       <c r="B1019" t="s">
-        <v>1978</v>
+        <v>1973</v>
       </c>
       <c r="C1019" t="s">
         <v>1792</v>
@@ -63861,7 +63792,7 @@
         <v>1794</v>
       </c>
       <c r="F1019" t="s">
-        <v>1795</v>
+        <v>136</v>
       </c>
       <c r="G1019" t="s">
         <v>41</v>
@@ -63902,22 +63833,22 @@
     </row>
     <row r="1020">
       <c r="A1020" t="s">
-        <v>1977</v>
+        <v>1972</v>
       </c>
       <c r="B1020" t="s">
-        <v>1978</v>
+        <v>1973</v>
       </c>
       <c r="C1020" t="s">
-        <v>1979</v>
+        <v>1974</v>
       </c>
       <c r="D1020" t="s">
-        <v>1980</v>
+        <v>1975</v>
       </c>
       <c r="E1020" t="s">
-        <v>1981</v>
+        <v>1976</v>
       </c>
       <c r="F1020" t="s">
-        <v>1976</v>
+        <v>118</v>
       </c>
       <c r="G1020" t="s">
         <v>24</v>
@@ -63958,22 +63889,22 @@
     </row>
     <row r="1021">
       <c r="A1021" t="s">
+        <v>1972</v>
+      </c>
+      <c r="B1021" t="s">
+        <v>1973</v>
+      </c>
+      <c r="C1021" t="s">
         <v>1977</v>
       </c>
-      <c r="B1021" t="s">
+      <c r="D1021" t="s">
         <v>1978</v>
       </c>
-      <c r="C1021" t="s">
-        <v>1982</v>
-      </c>
-      <c r="D1021" t="s">
-        <v>1983</v>
-      </c>
       <c r="E1021" t="s">
-        <v>1984</v>
+        <v>1979</v>
       </c>
       <c r="F1021" t="s">
-        <v>1962</v>
+        <v>70</v>
       </c>
       <c r="G1021" t="s">
         <v>24</v>
@@ -64014,10 +63945,10 @@
     </row>
     <row r="1022">
       <c r="A1022" t="s">
-        <v>1985</v>
+        <v>1980</v>
       </c>
       <c r="B1022" t="s">
-        <v>1986</v>
+        <v>1981</v>
       </c>
       <c r="C1022" t="s">
         <v>1792</v>
@@ -64029,7 +63960,7 @@
         <v>1794</v>
       </c>
       <c r="F1022" t="s">
-        <v>1795</v>
+        <v>136</v>
       </c>
       <c r="G1022" t="s">
         <v>41</v>
@@ -64070,22 +64001,22 @@
     </row>
     <row r="1023">
       <c r="A1023" t="s">
-        <v>1985</v>
+        <v>1980</v>
       </c>
       <c r="B1023" t="s">
-        <v>1986</v>
+        <v>1981</v>
       </c>
       <c r="C1023" t="s">
-        <v>1987</v>
+        <v>1982</v>
       </c>
       <c r="D1023" t="s">
-        <v>1988</v>
+        <v>1983</v>
       </c>
       <c r="E1023" t="s">
-        <v>1989</v>
+        <v>1984</v>
       </c>
       <c r="F1023" t="s">
-        <v>1990</v>
+        <v>80</v>
       </c>
       <c r="G1023" t="s">
         <v>24</v>
@@ -64126,22 +64057,22 @@
     </row>
     <row r="1024">
       <c r="A1024" t="s">
+        <v>1980</v>
+      </c>
+      <c r="B1024" t="s">
+        <v>1981</v>
+      </c>
+      <c r="C1024" t="s">
         <v>1985</v>
       </c>
-      <c r="B1024" t="s">
+      <c r="D1024" t="s">
         <v>1986</v>
       </c>
-      <c r="C1024" t="s">
-        <v>1991</v>
-      </c>
-      <c r="D1024" t="s">
-        <v>1992</v>
-      </c>
       <c r="E1024" t="s">
-        <v>1993</v>
+        <v>1987</v>
       </c>
       <c r="F1024" t="s">
-        <v>1994</v>
+        <v>476</v>
       </c>
       <c r="G1024" t="s">
         <v>24</v>
@@ -64182,10 +64113,10 @@
     </row>
     <row r="1025">
       <c r="A1025" t="s">
-        <v>1995</v>
+        <v>1988</v>
       </c>
       <c r="B1025" t="s">
-        <v>1996</v>
+        <v>1989</v>
       </c>
       <c r="C1025" t="s">
         <v>1792</v>
@@ -64197,7 +64128,7 @@
         <v>1794</v>
       </c>
       <c r="F1025" t="s">
-        <v>1795</v>
+        <v>136</v>
       </c>
       <c r="G1025" t="s">
         <v>41</v>
@@ -64238,22 +64169,22 @@
     </row>
     <row r="1026">
       <c r="A1026" t="s">
-        <v>1995</v>
+        <v>1988</v>
       </c>
       <c r="B1026" t="s">
-        <v>1996</v>
+        <v>1989</v>
       </c>
       <c r="C1026" t="s">
-        <v>1997</v>
+        <v>1990</v>
       </c>
       <c r="D1026" t="s">
-        <v>1998</v>
+        <v>1991</v>
       </c>
       <c r="E1026" t="s">
-        <v>1999</v>
+        <v>1992</v>
       </c>
       <c r="F1026" t="s">
-        <v>1962</v>
+        <v>70</v>
       </c>
       <c r="G1026" t="s">
         <v>24</v>
@@ -64294,22 +64225,22 @@
     </row>
     <row r="1027">
       <c r="A1027" t="s">
-        <v>1995</v>
+        <v>1988</v>
       </c>
       <c r="B1027" t="s">
-        <v>1996</v>
+        <v>1989</v>
       </c>
       <c r="C1027" t="s">
-        <v>2000</v>
+        <v>1993</v>
       </c>
       <c r="D1027" t="s">
-        <v>2001</v>
+        <v>1994</v>
       </c>
       <c r="E1027" t="s">
-        <v>1975</v>
+        <v>1971</v>
       </c>
       <c r="F1027" t="s">
-        <v>1976</v>
+        <v>118</v>
       </c>
       <c r="G1027" t="s">
         <v>24</v>
@@ -64350,10 +64281,10 @@
     </row>
     <row r="1028">
       <c r="A1028" t="s">
-        <v>2002</v>
+        <v>1995</v>
       </c>
       <c r="B1028" t="s">
-        <v>2003</v>
+        <v>1996</v>
       </c>
       <c r="C1028" t="s">
         <v>1792</v>
@@ -64365,7 +64296,7 @@
         <v>1794</v>
       </c>
       <c r="F1028" t="s">
-        <v>1795</v>
+        <v>136</v>
       </c>
       <c r="G1028" t="s">
         <v>41</v>
@@ -64406,22 +64337,22 @@
     </row>
     <row r="1029">
       <c r="A1029" t="s">
-        <v>2002</v>
+        <v>1995</v>
       </c>
       <c r="B1029" t="s">
-        <v>2003</v>
+        <v>1996</v>
       </c>
       <c r="C1029" t="s">
-        <v>2004</v>
+        <v>1997</v>
       </c>
       <c r="D1029" t="s">
-        <v>2005</v>
+        <v>1998</v>
       </c>
       <c r="E1029" t="s">
-        <v>2006</v>
+        <v>1999</v>
       </c>
       <c r="F1029" t="s">
-        <v>2007</v>
+        <v>558</v>
       </c>
       <c r="G1029" t="s">
         <v>24</v>
@@ -64462,22 +64393,22 @@
     </row>
     <row r="1030">
       <c r="A1030" t="s">
+        <v>1995</v>
+      </c>
+      <c r="B1030" t="s">
+        <v>1996</v>
+      </c>
+      <c r="C1030" t="s">
+        <v>2000</v>
+      </c>
+      <c r="D1030" t="s">
+        <v>2001</v>
+      </c>
+      <c r="E1030" t="s">
         <v>2002</v>
       </c>
-      <c r="B1030" t="s">
-        <v>2003</v>
-      </c>
-      <c r="C1030" t="s">
-        <v>2008</v>
-      </c>
-      <c r="D1030" t="s">
-        <v>2009</v>
-      </c>
-      <c r="E1030" t="s">
-        <v>2010</v>
-      </c>
       <c r="F1030" t="s">
-        <v>1962</v>
+        <v>70</v>
       </c>
       <c r="G1030" t="s">
         <v>24</v>
@@ -64518,10 +64449,10 @@
     </row>
     <row r="1031">
       <c r="A1031" t="s">
-        <v>2011</v>
+        <v>2003</v>
       </c>
       <c r="B1031" t="s">
-        <v>2012</v>
+        <v>2004</v>
       </c>
       <c r="C1031" t="s">
         <v>1792</v>
@@ -64533,7 +64464,7 @@
         <v>1794</v>
       </c>
       <c r="F1031" t="s">
-        <v>1795</v>
+        <v>136</v>
       </c>
       <c r="G1031" t="s">
         <v>41</v>
@@ -64574,22 +64505,22 @@
     </row>
     <row r="1032">
       <c r="A1032" t="s">
-        <v>2011</v>
+        <v>2003</v>
       </c>
       <c r="B1032" t="s">
-        <v>2012</v>
+        <v>2004</v>
       </c>
       <c r="C1032" t="s">
-        <v>2013</v>
+        <v>2005</v>
       </c>
       <c r="D1032" t="s">
-        <v>2014</v>
+        <v>2006</v>
       </c>
       <c r="E1032" t="s">
-        <v>2015</v>
+        <v>2007</v>
       </c>
       <c r="F1032" t="s">
-        <v>1976</v>
+        <v>118</v>
       </c>
       <c r="G1032" t="s">
         <v>24</v>
@@ -64630,22 +64561,22 @@
     </row>
     <row r="1033">
       <c r="A1033" t="s">
-        <v>2011</v>
+        <v>2003</v>
       </c>
       <c r="B1033" t="s">
-        <v>2012</v>
+        <v>2004</v>
       </c>
       <c r="C1033" t="s">
-        <v>2016</v>
+        <v>2008</v>
       </c>
       <c r="D1033" t="s">
-        <v>2017</v>
+        <v>2009</v>
       </c>
       <c r="E1033" t="s">
-        <v>2018</v>
+        <v>2010</v>
       </c>
       <c r="F1033" t="s">
-        <v>2019</v>
+        <v>100</v>
       </c>
       <c r="G1033" t="s">
         <v>24</v>
@@ -64686,10 +64617,10 @@
     </row>
     <row r="1034">
       <c r="A1034" t="s">
-        <v>2020</v>
+        <v>2011</v>
       </c>
       <c r="B1034" t="s">
-        <v>2021</v>
+        <v>2012</v>
       </c>
       <c r="C1034" t="s">
         <v>1792</v>
@@ -64701,7 +64632,7 @@
         <v>1794</v>
       </c>
       <c r="F1034" t="s">
-        <v>1795</v>
+        <v>136</v>
       </c>
       <c r="G1034" t="s">
         <v>41</v>
@@ -64742,22 +64673,22 @@
     </row>
     <row r="1035">
       <c r="A1035" t="s">
-        <v>2020</v>
+        <v>2011</v>
       </c>
       <c r="B1035" t="s">
-        <v>2021</v>
+        <v>2012</v>
       </c>
       <c r="C1035" t="s">
-        <v>2022</v>
+        <v>2013</v>
       </c>
       <c r="D1035" t="s">
-        <v>2023</v>
+        <v>2014</v>
       </c>
       <c r="E1035" t="s">
-        <v>2024</v>
+        <v>2015</v>
       </c>
       <c r="F1035" t="s">
-        <v>2025</v>
+        <v>139</v>
       </c>
       <c r="G1035" t="s">
         <v>24</v>
@@ -64798,22 +64729,22 @@
     </row>
     <row r="1036">
       <c r="A1036" t="s">
-        <v>2020</v>
+        <v>2011</v>
       </c>
       <c r="B1036" t="s">
-        <v>2021</v>
+        <v>2012</v>
       </c>
       <c r="C1036" t="s">
-        <v>2026</v>
+        <v>2016</v>
       </c>
       <c r="D1036" t="s">
-        <v>2027</v>
+        <v>2017</v>
       </c>
       <c r="E1036" t="s">
-        <v>2028</v>
+        <v>2018</v>
       </c>
       <c r="F1036" t="s">
-        <v>1966</v>
+        <v>90</v>
       </c>
       <c r="G1036" t="s">
         <v>24</v>
@@ -64854,10 +64785,10 @@
     </row>
     <row r="1037">
       <c r="A1037" t="s">
-        <v>2029</v>
+        <v>2019</v>
       </c>
       <c r="B1037" t="s">
-        <v>2030</v>
+        <v>2020</v>
       </c>
       <c r="C1037" t="s">
         <v>1792</v>
@@ -64869,7 +64800,7 @@
         <v>1794</v>
       </c>
       <c r="F1037" t="s">
-        <v>1795</v>
+        <v>136</v>
       </c>
       <c r="G1037" t="s">
         <v>41</v>
@@ -64910,22 +64841,22 @@
     </row>
     <row r="1038">
       <c r="A1038" t="s">
-        <v>2029</v>
+        <v>2019</v>
       </c>
       <c r="B1038" t="s">
-        <v>2030</v>
+        <v>2020</v>
       </c>
       <c r="C1038" t="s">
-        <v>2031</v>
+        <v>2021</v>
       </c>
       <c r="D1038" t="s">
-        <v>2032</v>
+        <v>2022</v>
       </c>
       <c r="E1038" t="s">
-        <v>2033</v>
+        <v>2023</v>
       </c>
       <c r="F1038" t="s">
-        <v>2034</v>
+        <v>234</v>
       </c>
       <c r="G1038" t="s">
         <v>24</v>
@@ -64966,22 +64897,22 @@
     </row>
     <row r="1039">
       <c r="A1039" t="s">
-        <v>2029</v>
+        <v>2019</v>
       </c>
       <c r="B1039" t="s">
-        <v>2030</v>
+        <v>2020</v>
       </c>
       <c r="C1039" t="s">
-        <v>2035</v>
+        <v>2024</v>
       </c>
       <c r="D1039" t="s">
-        <v>2036</v>
+        <v>2025</v>
       </c>
       <c r="E1039" t="s">
-        <v>2037</v>
+        <v>2026</v>
       </c>
       <c r="F1039" t="s">
-        <v>2038</v>
+        <v>94</v>
       </c>
       <c r="G1039" t="s">
         <v>24</v>
@@ -65022,10 +64953,10 @@
     </row>
     <row r="1040">
       <c r="A1040" t="s">
-        <v>2039</v>
+        <v>2027</v>
       </c>
       <c r="B1040" t="s">
-        <v>2040</v>
+        <v>2028</v>
       </c>
       <c r="C1040" t="s">
         <v>1792</v>
@@ -65037,7 +64968,7 @@
         <v>1794</v>
       </c>
       <c r="F1040" t="s">
-        <v>1795</v>
+        <v>136</v>
       </c>
       <c r="G1040" t="s">
         <v>41</v>
@@ -65078,22 +65009,22 @@
     </row>
     <row r="1041">
       <c r="A1041" t="s">
-        <v>2039</v>
+        <v>2027</v>
       </c>
       <c r="B1041" t="s">
-        <v>2040</v>
+        <v>2028</v>
       </c>
       <c r="C1041" t="s">
-        <v>2041</v>
+        <v>2029</v>
       </c>
       <c r="D1041" t="s">
-        <v>2042</v>
+        <v>2030</v>
       </c>
       <c r="E1041" t="s">
-        <v>2043</v>
+        <v>2031</v>
       </c>
       <c r="F1041" t="s">
-        <v>2044</v>
+        <v>54</v>
       </c>
       <c r="G1041" t="s">
         <v>24</v>
@@ -65134,22 +65065,22 @@
     </row>
     <row r="1042">
       <c r="A1042" t="s">
-        <v>2039</v>
+        <v>2027</v>
       </c>
       <c r="B1042" t="s">
-        <v>2040</v>
+        <v>2028</v>
       </c>
       <c r="C1042" t="s">
-        <v>2045</v>
+        <v>2032</v>
       </c>
       <c r="D1042" t="s">
-        <v>2046</v>
+        <v>2033</v>
       </c>
       <c r="E1042" t="s">
-        <v>2047</v>
+        <v>2034</v>
       </c>
       <c r="F1042" t="s">
-        <v>1972</v>
+        <v>209</v>
       </c>
       <c r="G1042" t="s">
         <v>24</v>
@@ -65190,22 +65121,22 @@
     </row>
     <row r="1043">
       <c r="A1043" t="s">
-        <v>2048</v>
+        <v>2035</v>
       </c>
       <c r="B1043" t="s">
-        <v>2049</v>
+        <v>2036</v>
       </c>
       <c r="C1043" t="s">
-        <v>2050</v>
+        <v>2037</v>
       </c>
       <c r="D1043" t="s">
-        <v>2051</v>
+        <v>2038</v>
       </c>
       <c r="E1043" t="s">
-        <v>2052</v>
+        <v>2039</v>
       </c>
       <c r="F1043" t="s">
-        <v>2053</v>
+        <v>23</v>
       </c>
       <c r="G1043" t="s">
         <v>24</v>
@@ -65246,22 +65177,22 @@
     </row>
     <row r="1044">
       <c r="A1044" t="s">
-        <v>2048</v>
+        <v>2035</v>
       </c>
       <c r="B1044" t="s">
-        <v>2049</v>
+        <v>2036</v>
       </c>
       <c r="C1044" t="s">
-        <v>2054</v>
+        <v>2040</v>
       </c>
       <c r="D1044" t="s">
-        <v>2055</v>
+        <v>2041</v>
       </c>
       <c r="E1044" t="s">
-        <v>2056</v>
+        <v>2042</v>
       </c>
       <c r="F1044" t="s">
-        <v>2057</v>
+        <v>64</v>
       </c>
       <c r="G1044" t="s">
         <v>24</v>
@@ -65302,10 +65233,10 @@
     </row>
     <row r="1045">
       <c r="A1045" t="s">
-        <v>2048</v>
+        <v>2035</v>
       </c>
       <c r="B1045" t="s">
-        <v>2049</v>
+        <v>2036</v>
       </c>
       <c r="C1045" t="s">
         <v>1792</v>
@@ -65317,7 +65248,7 @@
         <v>1794</v>
       </c>
       <c r="F1045" t="s">
-        <v>1795</v>
+        <v>136</v>
       </c>
       <c r="G1045" t="s">
         <v>41</v>
@@ -65358,22 +65289,22 @@
     </row>
     <row r="1046">
       <c r="A1046" t="s">
-        <v>2058</v>
+        <v>2043</v>
       </c>
       <c r="B1046" t="s">
-        <v>2059</v>
+        <v>2044</v>
       </c>
       <c r="C1046" t="s">
-        <v>2050</v>
+        <v>2037</v>
       </c>
       <c r="D1046" t="s">
-        <v>2051</v>
+        <v>2038</v>
       </c>
       <c r="E1046" t="s">
-        <v>2052</v>
+        <v>2039</v>
       </c>
       <c r="F1046" t="s">
-        <v>2053</v>
+        <v>23</v>
       </c>
       <c r="G1046" t="s">
         <v>41</v>
@@ -65414,22 +65345,22 @@
     </row>
     <row r="1047">
       <c r="A1047" t="s">
-        <v>2058</v>
+        <v>2043</v>
       </c>
       <c r="B1047" t="s">
-        <v>2059</v>
+        <v>2044</v>
       </c>
       <c r="C1047" t="s">
-        <v>2060</v>
+        <v>2045</v>
       </c>
       <c r="D1047" t="s">
-        <v>2061</v>
+        <v>2046</v>
       </c>
       <c r="E1047" t="s">
-        <v>2062</v>
+        <v>2047</v>
       </c>
       <c r="F1047" t="s">
-        <v>2063</v>
+        <v>785</v>
       </c>
       <c r="G1047" t="s">
         <v>24</v>
@@ -65470,22 +65401,22 @@
     </row>
     <row r="1048">
       <c r="A1048" t="s">
-        <v>2058</v>
+        <v>2043</v>
       </c>
       <c r="B1048" t="s">
-        <v>2059</v>
+        <v>2044</v>
       </c>
       <c r="C1048" t="s">
-        <v>2064</v>
+        <v>2048</v>
       </c>
       <c r="D1048" t="s">
-        <v>2065</v>
+        <v>2049</v>
       </c>
       <c r="E1048" t="s">
-        <v>2066</v>
+        <v>2050</v>
       </c>
       <c r="F1048" t="s">
-        <v>1976</v>
+        <v>118</v>
       </c>
       <c r="G1048" t="s">
         <v>24</v>
@@ -65526,22 +65457,22 @@
     </row>
     <row r="1049">
       <c r="A1049" t="s">
-        <v>2067</v>
+        <v>2051</v>
       </c>
       <c r="B1049" t="s">
-        <v>2068</v>
+        <v>2052</v>
       </c>
       <c r="C1049" t="s">
-        <v>2050</v>
+        <v>2037</v>
       </c>
       <c r="D1049" t="s">
-        <v>2051</v>
+        <v>2038</v>
       </c>
       <c r="E1049" t="s">
-        <v>2052</v>
+        <v>2039</v>
       </c>
       <c r="F1049" t="s">
-        <v>2053</v>
+        <v>23</v>
       </c>
       <c r="G1049" t="s">
         <v>41</v>
@@ -65582,22 +65513,22 @@
     </row>
     <row r="1050">
       <c r="A1050" t="s">
-        <v>2067</v>
+        <v>2051</v>
       </c>
       <c r="B1050" t="s">
-        <v>2068</v>
+        <v>2052</v>
       </c>
       <c r="C1050" t="s">
-        <v>2069</v>
+        <v>2053</v>
       </c>
       <c r="D1050" t="s">
-        <v>2070</v>
+        <v>2054</v>
       </c>
       <c r="E1050" t="s">
-        <v>2071</v>
+        <v>2055</v>
       </c>
       <c r="F1050" t="s">
-        <v>1976</v>
+        <v>118</v>
       </c>
       <c r="G1050" t="s">
         <v>24</v>
@@ -65638,22 +65569,22 @@
     </row>
     <row r="1051">
       <c r="A1051" t="s">
-        <v>2067</v>
+        <v>2051</v>
       </c>
       <c r="B1051" t="s">
-        <v>2068</v>
+        <v>2052</v>
       </c>
       <c r="C1051" t="s">
-        <v>2072</v>
+        <v>2056</v>
       </c>
       <c r="D1051" t="s">
-        <v>2073</v>
+        <v>2057</v>
       </c>
       <c r="E1051" t="s">
-        <v>2074</v>
+        <v>2058</v>
       </c>
       <c r="F1051" t="s">
-        <v>2075</v>
+        <v>2059</v>
       </c>
       <c r="G1051" t="s">
         <v>24</v>
@@ -65694,22 +65625,22 @@
     </row>
     <row r="1052">
       <c r="A1052" t="s">
-        <v>2076</v>
+        <v>2060</v>
       </c>
       <c r="B1052" t="s">
-        <v>2077</v>
+        <v>2061</v>
       </c>
       <c r="C1052" t="s">
-        <v>2050</v>
+        <v>2037</v>
       </c>
       <c r="D1052" t="s">
-        <v>2051</v>
+        <v>2038</v>
       </c>
       <c r="E1052" t="s">
-        <v>2052</v>
+        <v>2039</v>
       </c>
       <c r="F1052" t="s">
-        <v>2053</v>
+        <v>23</v>
       </c>
       <c r="G1052" t="s">
         <v>41</v>
@@ -65750,22 +65681,22 @@
     </row>
     <row r="1053">
       <c r="A1053" t="s">
-        <v>2076</v>
+        <v>2060</v>
       </c>
       <c r="B1053" t="s">
-        <v>2077</v>
+        <v>2061</v>
       </c>
       <c r="C1053" t="s">
-        <v>2078</v>
+        <v>2062</v>
       </c>
       <c r="D1053" t="s">
-        <v>2079</v>
+        <v>2063</v>
       </c>
       <c r="E1053" t="s">
-        <v>2080</v>
+        <v>2064</v>
       </c>
       <c r="F1053" t="s">
-        <v>1795</v>
+        <v>136</v>
       </c>
       <c r="G1053" t="s">
         <v>24</v>
@@ -65806,22 +65737,22 @@
     </row>
     <row r="1054">
       <c r="A1054" t="s">
-        <v>2076</v>
+        <v>2060</v>
       </c>
       <c r="B1054" t="s">
-        <v>2077</v>
+        <v>2061</v>
       </c>
       <c r="C1054" t="s">
-        <v>2081</v>
+        <v>2065</v>
       </c>
       <c r="D1054" t="s">
-        <v>2082</v>
+        <v>2066</v>
       </c>
       <c r="E1054" t="s">
-        <v>2083</v>
+        <v>2067</v>
       </c>
       <c r="F1054" t="s">
-        <v>1795</v>
+        <v>136</v>
       </c>
       <c r="G1054" t="s">
         <v>24</v>
@@ -65862,22 +65793,22 @@
     </row>
     <row r="1055">
       <c r="A1055" t="s">
-        <v>2084</v>
+        <v>2068</v>
       </c>
       <c r="B1055" t="s">
-        <v>2085</v>
+        <v>2069</v>
       </c>
       <c r="C1055" t="s">
-        <v>2086</v>
+        <v>2070</v>
       </c>
       <c r="D1055" t="s">
-        <v>2087</v>
+        <v>2071</v>
       </c>
       <c r="E1055" t="s">
-        <v>2088</v>
+        <v>2072</v>
       </c>
       <c r="F1055" t="s">
-        <v>2089</v>
+        <v>262</v>
       </c>
       <c r="G1055" t="s">
         <v>24</v>
@@ -65918,22 +65849,22 @@
     </row>
     <row r="1056">
       <c r="A1056" t="s">
-        <v>2084</v>
+        <v>2068</v>
       </c>
       <c r="B1056" t="s">
-        <v>2085</v>
+        <v>2069</v>
       </c>
       <c r="C1056" t="s">
-        <v>2090</v>
+        <v>2073</v>
       </c>
       <c r="D1056" t="s">
-        <v>2091</v>
+        <v>2074</v>
       </c>
       <c r="E1056" t="s">
-        <v>2092</v>
+        <v>2075</v>
       </c>
       <c r="F1056" t="s">
-        <v>2093</v>
+        <v>74</v>
       </c>
       <c r="G1056" t="s">
         <v>24</v>
@@ -65974,22 +65905,22 @@
     </row>
     <row r="1057">
       <c r="A1057" t="s">
-        <v>2084</v>
+        <v>2068</v>
       </c>
       <c r="B1057" t="s">
-        <v>2085</v>
+        <v>2069</v>
       </c>
       <c r="C1057" t="s">
-        <v>2050</v>
+        <v>2037</v>
       </c>
       <c r="D1057" t="s">
-        <v>2051</v>
+        <v>2038</v>
       </c>
       <c r="E1057" t="s">
-        <v>2052</v>
+        <v>2039</v>
       </c>
       <c r="F1057" t="s">
-        <v>2053</v>
+        <v>23</v>
       </c>
       <c r="G1057" t="s">
         <v>41</v>
@@ -66030,22 +65961,22 @@
     </row>
     <row r="1058">
       <c r="A1058" t="s">
-        <v>2094</v>
+        <v>2076</v>
       </c>
       <c r="B1058" t="s">
-        <v>2095</v>
+        <v>2077</v>
       </c>
       <c r="C1058" t="s">
-        <v>2086</v>
+        <v>2070</v>
       </c>
       <c r="D1058" t="s">
-        <v>2087</v>
+        <v>2071</v>
       </c>
       <c r="E1058" t="s">
-        <v>2088</v>
+        <v>2072</v>
       </c>
       <c r="F1058" t="s">
-        <v>2089</v>
+        <v>262</v>
       </c>
       <c r="G1058" t="s">
         <v>41</v>
@@ -66086,22 +66017,22 @@
     </row>
     <row r="1059">
       <c r="A1059" t="s">
-        <v>2094</v>
+        <v>2076</v>
       </c>
       <c r="B1059" t="s">
-        <v>2095</v>
+        <v>2077</v>
       </c>
       <c r="C1059" t="s">
-        <v>2096</v>
+        <v>2078</v>
       </c>
       <c r="D1059" t="s">
-        <v>2046</v>
+        <v>2033</v>
       </c>
       <c r="E1059" t="s">
-        <v>2010</v>
+        <v>2002</v>
       </c>
       <c r="F1059" t="s">
-        <v>1962</v>
+        <v>70</v>
       </c>
       <c r="G1059" t="s">
         <v>24</v>
@@ -66142,22 +66073,22 @@
     </row>
     <row r="1060">
       <c r="A1060" t="s">
-        <v>2094</v>
+        <v>2076</v>
       </c>
       <c r="B1060" t="s">
-        <v>2095</v>
+        <v>2077</v>
       </c>
       <c r="C1060" t="s">
-        <v>2097</v>
+        <v>2079</v>
       </c>
       <c r="D1060" t="s">
-        <v>2098</v>
+        <v>2080</v>
       </c>
       <c r="E1060" t="s">
-        <v>2099</v>
+        <v>2081</v>
       </c>
       <c r="F1060" t="s">
-        <v>1976</v>
+        <v>118</v>
       </c>
       <c r="G1060" t="s">
         <v>24</v>
@@ -66198,22 +66129,22 @@
     </row>
     <row r="1061">
       <c r="A1061" t="s">
-        <v>2100</v>
+        <v>2082</v>
       </c>
       <c r="B1061" t="s">
-        <v>2101</v>
+        <v>2083</v>
       </c>
       <c r="C1061" t="s">
-        <v>2102</v>
+        <v>2084</v>
       </c>
       <c r="D1061" t="s">
-        <v>2103</v>
+        <v>2085</v>
       </c>
       <c r="E1061" t="s">
-        <v>2104</v>
+        <v>2086</v>
       </c>
       <c r="F1061" t="s">
-        <v>2053</v>
+        <v>23</v>
       </c>
       <c r="G1061" t="s">
         <v>24</v>
@@ -66254,22 +66185,22 @@
     </row>
     <row r="1062">
       <c r="A1062" t="s">
-        <v>2100</v>
+        <v>2082</v>
       </c>
       <c r="B1062" t="s">
-        <v>2101</v>
+        <v>2083</v>
       </c>
       <c r="C1062" t="s">
-        <v>2105</v>
+        <v>2087</v>
       </c>
       <c r="D1062" t="s">
-        <v>2106</v>
+        <v>2088</v>
       </c>
       <c r="E1062" t="s">
-        <v>2066</v>
+        <v>2050</v>
       </c>
       <c r="F1062" t="s">
-        <v>1976</v>
+        <v>118</v>
       </c>
       <c r="G1062" t="s">
         <v>24</v>
@@ -66310,22 +66241,22 @@
     </row>
     <row r="1063">
       <c r="A1063" t="s">
-        <v>2100</v>
+        <v>2082</v>
       </c>
       <c r="B1063" t="s">
-        <v>2101</v>
+        <v>2083</v>
       </c>
       <c r="C1063" t="s">
-        <v>2086</v>
+        <v>2070</v>
       </c>
       <c r="D1063" t="s">
-        <v>2087</v>
+        <v>2071</v>
       </c>
       <c r="E1063" t="s">
-        <v>2088</v>
+        <v>2072</v>
       </c>
       <c r="F1063" t="s">
-        <v>2089</v>
+        <v>262</v>
       </c>
       <c r="G1063" t="s">
         <v>41</v>
@@ -66366,22 +66297,22 @@
     </row>
     <row r="1064">
       <c r="A1064" t="s">
-        <v>2107</v>
+        <v>2089</v>
       </c>
       <c r="B1064" t="s">
-        <v>2108</v>
+        <v>2090</v>
       </c>
       <c r="C1064" t="s">
-        <v>2109</v>
+        <v>2091</v>
       </c>
       <c r="D1064" t="s">
-        <v>2110</v>
+        <v>2092</v>
       </c>
       <c r="E1064" t="s">
-        <v>2111</v>
+        <v>2093</v>
       </c>
       <c r="F1064" t="s">
-        <v>2112</v>
+        <v>84</v>
       </c>
       <c r="G1064" t="s">
         <v>24</v>
@@ -66422,22 +66353,22 @@
     </row>
     <row r="1065">
       <c r="A1065" t="s">
-        <v>2107</v>
+        <v>2089</v>
       </c>
       <c r="B1065" t="s">
-        <v>2108</v>
+        <v>2090</v>
       </c>
       <c r="C1065" t="s">
-        <v>2113</v>
+        <v>2094</v>
       </c>
       <c r="D1065" t="s">
-        <v>2114</v>
+        <v>2095</v>
       </c>
       <c r="E1065" t="s">
-        <v>2115</v>
+        <v>2096</v>
       </c>
       <c r="F1065" t="s">
-        <v>2057</v>
+        <v>64</v>
       </c>
       <c r="G1065" t="s">
         <v>24</v>
@@ -66478,22 +66409,22 @@
     </row>
     <row r="1066">
       <c r="A1066" t="s">
-        <v>2107</v>
+        <v>2089</v>
       </c>
       <c r="B1066" t="s">
-        <v>2108</v>
+        <v>2090</v>
       </c>
       <c r="C1066" t="s">
-        <v>2102</v>
+        <v>2084</v>
       </c>
       <c r="D1066" t="s">
-        <v>2103</v>
+        <v>2085</v>
       </c>
       <c r="E1066" t="s">
-        <v>2104</v>
+        <v>2086</v>
       </c>
       <c r="F1066" t="s">
-        <v>2053</v>
+        <v>23</v>
       </c>
       <c r="G1066" t="s">
         <v>41</v>
@@ -66534,22 +66465,22 @@
     </row>
     <row r="1067">
       <c r="A1067" t="s">
-        <v>2116</v>
+        <v>2097</v>
       </c>
       <c r="B1067" t="s">
-        <v>2117</v>
+        <v>2098</v>
       </c>
       <c r="C1067" t="s">
-        <v>2109</v>
+        <v>2091</v>
       </c>
       <c r="D1067" t="s">
-        <v>2110</v>
+        <v>2092</v>
       </c>
       <c r="E1067" t="s">
-        <v>2111</v>
+        <v>2093</v>
       </c>
       <c r="F1067" t="s">
-        <v>2112</v>
+        <v>84</v>
       </c>
       <c r="G1067" t="s">
         <v>41</v>
@@ -66590,22 +66521,22 @@
     </row>
     <row r="1068">
       <c r="A1068" t="s">
-        <v>2116</v>
+        <v>2097</v>
       </c>
       <c r="B1068" t="s">
-        <v>2117</v>
+        <v>2098</v>
       </c>
       <c r="C1068" t="s">
-        <v>2118</v>
+        <v>2099</v>
       </c>
       <c r="D1068" t="s">
-        <v>2119</v>
+        <v>2100</v>
       </c>
       <c r="E1068" t="s">
-        <v>2120</v>
+        <v>2101</v>
       </c>
       <c r="F1068" t="s">
-        <v>1972</v>
+        <v>209</v>
       </c>
       <c r="G1068" t="s">
         <v>24</v>
@@ -66646,22 +66577,22 @@
     </row>
     <row r="1069">
       <c r="A1069" t="s">
-        <v>2116</v>
+        <v>2097</v>
       </c>
       <c r="B1069" t="s">
-        <v>2117</v>
+        <v>2098</v>
       </c>
       <c r="C1069" t="s">
-        <v>2121</v>
+        <v>2102</v>
       </c>
       <c r="D1069" t="s">
-        <v>2122</v>
+        <v>2103</v>
       </c>
       <c r="E1069" t="s">
-        <v>2123</v>
+        <v>2104</v>
       </c>
       <c r="F1069" t="s">
-        <v>2093</v>
+        <v>74</v>
       </c>
       <c r="G1069" t="s">
         <v>24</v>
@@ -66702,22 +66633,22 @@
     </row>
     <row r="1070">
       <c r="A1070" t="s">
-        <v>2124</v>
+        <v>2105</v>
       </c>
       <c r="B1070" t="s">
-        <v>2125</v>
+        <v>2106</v>
       </c>
       <c r="C1070" t="s">
-        <v>2109</v>
+        <v>2091</v>
       </c>
       <c r="D1070" t="s">
-        <v>2110</v>
+        <v>2092</v>
       </c>
       <c r="E1070" t="s">
-        <v>2111</v>
+        <v>2093</v>
       </c>
       <c r="F1070" t="s">
-        <v>2112</v>
+        <v>84</v>
       </c>
       <c r="G1070" t="s">
         <v>41</v>
@@ -66758,22 +66689,22 @@
     </row>
     <row r="1071">
       <c r="A1071" t="s">
-        <v>2124</v>
+        <v>2105</v>
       </c>
       <c r="B1071" t="s">
-        <v>2125</v>
+        <v>2106</v>
       </c>
       <c r="C1071" t="s">
-        <v>2126</v>
+        <v>2107</v>
       </c>
       <c r="D1071" t="s">
-        <v>2127</v>
+        <v>2108</v>
       </c>
       <c r="E1071" t="s">
-        <v>1975</v>
+        <v>1971</v>
       </c>
       <c r="F1071" t="s">
-        <v>1976</v>
+        <v>118</v>
       </c>
       <c r="G1071" t="s">
         <v>24</v>
@@ -66814,22 +66745,22 @@
     </row>
     <row r="1072">
       <c r="A1072" t="s">
-        <v>2124</v>
+        <v>2105</v>
       </c>
       <c r="B1072" t="s">
-        <v>2125</v>
+        <v>2106</v>
       </c>
       <c r="C1072" t="s">
-        <v>2128</v>
+        <v>2109</v>
       </c>
       <c r="D1072" t="s">
-        <v>2129</v>
+        <v>2110</v>
       </c>
       <c r="E1072" t="s">
-        <v>2130</v>
+        <v>2111</v>
       </c>
       <c r="F1072" t="s">
-        <v>2038</v>
+        <v>94</v>
       </c>
       <c r="G1072" t="s">
         <v>24</v>
@@ -66870,22 +66801,22 @@
     </row>
     <row r="1073">
       <c r="A1073" t="s">
-        <v>2131</v>
+        <v>2112</v>
       </c>
       <c r="B1073" t="s">
-        <v>2132</v>
+        <v>2113</v>
       </c>
       <c r="C1073" t="s">
-        <v>2133</v>
+        <v>2114</v>
       </c>
       <c r="D1073" t="s">
-        <v>2134</v>
+        <v>2115</v>
       </c>
       <c r="E1073" t="s">
-        <v>2135</v>
+        <v>2116</v>
       </c>
       <c r="F1073" t="s">
-        <v>2136</v>
+        <v>40</v>
       </c>
       <c r="G1073" t="s">
         <v>24</v>
@@ -66926,22 +66857,22 @@
     </row>
     <row r="1074">
       <c r="A1074" t="s">
-        <v>2131</v>
+        <v>2112</v>
       </c>
       <c r="B1074" t="s">
-        <v>2132</v>
+        <v>2113</v>
       </c>
       <c r="C1074" t="s">
-        <v>2137</v>
+        <v>2117</v>
       </c>
       <c r="D1074" t="s">
-        <v>2138</v>
+        <v>2118</v>
       </c>
       <c r="E1074" t="s">
-        <v>2139</v>
+        <v>2119</v>
       </c>
       <c r="F1074" t="s">
-        <v>2140</v>
+        <v>1291</v>
       </c>
       <c r="G1074" t="s">
         <v>24</v>
@@ -66982,22 +66913,22 @@
     </row>
     <row r="1075">
       <c r="A1075" t="s">
-        <v>2131</v>
+        <v>2112</v>
       </c>
       <c r="B1075" t="s">
-        <v>2132</v>
+        <v>2113</v>
       </c>
       <c r="C1075" t="s">
-        <v>2109</v>
+        <v>2091</v>
       </c>
       <c r="D1075" t="s">
-        <v>2110</v>
+        <v>2092</v>
       </c>
       <c r="E1075" t="s">
-        <v>2111</v>
+        <v>2093</v>
       </c>
       <c r="F1075" t="s">
-        <v>2112</v>
+        <v>84</v>
       </c>
       <c r="G1075" t="s">
         <v>41</v>
@@ -67038,22 +66969,22 @@
     </row>
     <row r="1076">
       <c r="A1076" t="s">
-        <v>2141</v>
+        <v>2120</v>
       </c>
       <c r="B1076" t="s">
-        <v>2142</v>
+        <v>2121</v>
       </c>
       <c r="C1076" t="s">
-        <v>2133</v>
+        <v>2114</v>
       </c>
       <c r="D1076" t="s">
-        <v>2134</v>
+        <v>2115</v>
       </c>
       <c r="E1076" t="s">
-        <v>2135</v>
+        <v>2116</v>
       </c>
       <c r="F1076" t="s">
-        <v>2136</v>
+        <v>40</v>
       </c>
       <c r="G1076" t="s">
         <v>41</v>
@@ -67094,22 +67025,22 @@
     </row>
     <row r="1077">
       <c r="A1077" t="s">
-        <v>2141</v>
+        <v>2120</v>
       </c>
       <c r="B1077" t="s">
-        <v>2142</v>
+        <v>2121</v>
       </c>
       <c r="C1077" t="s">
-        <v>2143</v>
+        <v>2122</v>
       </c>
       <c r="D1077" t="s">
-        <v>2144</v>
+        <v>2123</v>
       </c>
       <c r="E1077" t="s">
-        <v>2013</v>
+        <v>2005</v>
       </c>
       <c r="F1077" t="s">
-        <v>2145</v>
+        <v>60</v>
       </c>
       <c r="G1077" t="s">
         <v>24</v>
@@ -67150,22 +67081,22 @@
     </row>
     <row r="1078">
       <c r="A1078" t="s">
-        <v>2141</v>
+        <v>2120</v>
       </c>
       <c r="B1078" t="s">
-        <v>2142</v>
+        <v>2121</v>
       </c>
       <c r="C1078" t="s">
-        <v>2146</v>
+        <v>2124</v>
       </c>
       <c r="D1078" t="s">
-        <v>2147</v>
+        <v>2125</v>
       </c>
       <c r="E1078" t="s">
-        <v>2066</v>
+        <v>2050</v>
       </c>
       <c r="F1078" t="s">
-        <v>1976</v>
+        <v>118</v>
       </c>
       <c r="G1078" t="s">
         <v>24</v>
@@ -67206,22 +67137,22 @@
     </row>
     <row r="1079">
       <c r="A1079" t="s">
-        <v>2148</v>
+        <v>2126</v>
       </c>
       <c r="B1079" t="s">
-        <v>2149</v>
+        <v>2127</v>
       </c>
       <c r="C1079" t="s">
-        <v>2133</v>
+        <v>2114</v>
       </c>
       <c r="D1079" t="s">
-        <v>2134</v>
+        <v>2115</v>
       </c>
       <c r="E1079" t="s">
-        <v>2135</v>
+        <v>2116</v>
       </c>
       <c r="F1079" t="s">
-        <v>2136</v>
+        <v>40</v>
       </c>
       <c r="G1079" t="s">
         <v>41</v>
@@ -67262,22 +67193,22 @@
     </row>
     <row r="1080">
       <c r="A1080" t="s">
-        <v>2148</v>
+        <v>2126</v>
       </c>
       <c r="B1080" t="s">
-        <v>2149</v>
+        <v>2127</v>
       </c>
       <c r="C1080" t="s">
-        <v>2150</v>
+        <v>2128</v>
       </c>
       <c r="D1080" t="s">
-        <v>2151</v>
+        <v>2129</v>
       </c>
       <c r="E1080" t="s">
-        <v>2006</v>
+        <v>1999</v>
       </c>
       <c r="F1080" t="s">
-        <v>2007</v>
+        <v>558</v>
       </c>
       <c r="G1080" t="s">
         <v>24</v>
@@ -67318,22 +67249,22 @@
     </row>
     <row r="1081">
       <c r="A1081" t="s">
-        <v>2148</v>
+        <v>2126</v>
       </c>
       <c r="B1081" t="s">
-        <v>2149</v>
+        <v>2127</v>
       </c>
       <c r="C1081" t="s">
-        <v>2152</v>
+        <v>2130</v>
       </c>
       <c r="D1081" t="s">
-        <v>2153</v>
+        <v>2131</v>
       </c>
       <c r="E1081" t="s">
-        <v>2154</v>
+        <v>2132</v>
       </c>
       <c r="F1081" t="s">
-        <v>2145</v>
+        <v>60</v>
       </c>
       <c r="G1081" t="s">
         <v>24</v>
@@ -67374,22 +67305,22 @@
     </row>
     <row r="1082">
       <c r="A1082" t="s">
-        <v>2155</v>
+        <v>2133</v>
       </c>
       <c r="B1082" t="s">
-        <v>2156</v>
+        <v>2134</v>
       </c>
       <c r="C1082" t="s">
-        <v>2133</v>
+        <v>2114</v>
       </c>
       <c r="D1082" t="s">
-        <v>2134</v>
+        <v>2115</v>
       </c>
       <c r="E1082" t="s">
-        <v>2135</v>
+        <v>2116</v>
       </c>
       <c r="F1082" t="s">
-        <v>2136</v>
+        <v>40</v>
       </c>
       <c r="G1082" t="s">
         <v>41</v>
@@ -67430,22 +67361,22 @@
     </row>
     <row r="1083">
       <c r="A1083" t="s">
-        <v>2155</v>
+        <v>2133</v>
       </c>
       <c r="B1083" t="s">
-        <v>2156</v>
+        <v>2134</v>
       </c>
       <c r="C1083" t="s">
-        <v>2157</v>
+        <v>2135</v>
       </c>
       <c r="D1083" t="s">
-        <v>2158</v>
+        <v>2136</v>
       </c>
       <c r="E1083" t="s">
-        <v>1999</v>
+        <v>1992</v>
       </c>
       <c r="F1083" t="s">
-        <v>1962</v>
+        <v>70</v>
       </c>
       <c r="G1083" t="s">
         <v>24</v>
@@ -67486,22 +67417,22 @@
     </row>
     <row r="1084">
       <c r="A1084" t="s">
-        <v>2155</v>
+        <v>2133</v>
       </c>
       <c r="B1084" t="s">
-        <v>2156</v>
+        <v>2134</v>
       </c>
       <c r="C1084" t="s">
-        <v>2159</v>
+        <v>2137</v>
       </c>
       <c r="D1084" t="s">
-        <v>2160</v>
+        <v>2138</v>
       </c>
       <c r="E1084" t="s">
-        <v>2161</v>
+        <v>2139</v>
       </c>
       <c r="F1084" t="s">
-        <v>2162</v>
+        <v>363</v>
       </c>
       <c r="G1084" t="s">
         <v>24</v>
@@ -67542,22 +67473,22 @@
     </row>
     <row r="1085">
       <c r="A1085" t="s">
-        <v>2163</v>
+        <v>2140</v>
       </c>
       <c r="B1085" t="s">
-        <v>2164</v>
+        <v>2141</v>
       </c>
       <c r="C1085" t="s">
-        <v>2133</v>
+        <v>2114</v>
       </c>
       <c r="D1085" t="s">
-        <v>2134</v>
+        <v>2115</v>
       </c>
       <c r="E1085" t="s">
-        <v>2135</v>
+        <v>2116</v>
       </c>
       <c r="F1085" t="s">
-        <v>2136</v>
+        <v>40</v>
       </c>
       <c r="G1085" t="s">
         <v>41</v>
@@ -67598,22 +67529,22 @@
     </row>
     <row r="1086">
       <c r="A1086" t="s">
-        <v>2163</v>
+        <v>2140</v>
       </c>
       <c r="B1086" t="s">
-        <v>2164</v>
+        <v>2141</v>
       </c>
       <c r="C1086" t="s">
-        <v>2165</v>
+        <v>2142</v>
       </c>
       <c r="D1086" t="s">
-        <v>2166</v>
+        <v>2143</v>
       </c>
       <c r="E1086" t="s">
-        <v>2167</v>
+        <v>2144</v>
       </c>
       <c r="F1086" t="s">
-        <v>2025</v>
+        <v>139</v>
       </c>
       <c r="G1086" t="s">
         <v>24</v>
@@ -67654,22 +67585,22 @@
     </row>
     <row r="1087">
       <c r="A1087" t="s">
-        <v>2163</v>
+        <v>2140</v>
       </c>
       <c r="B1087" t="s">
-        <v>2164</v>
+        <v>2141</v>
       </c>
       <c r="C1087" t="s">
-        <v>2168</v>
+        <v>2145</v>
       </c>
       <c r="D1087" t="s">
-        <v>2169</v>
+        <v>2146</v>
       </c>
       <c r="E1087" t="s">
-        <v>2170</v>
+        <v>2147</v>
       </c>
       <c r="F1087" t="s">
-        <v>2057</v>
+        <v>64</v>
       </c>
       <c r="G1087" t="s">
         <v>24</v>

</xml_diff>